<commit_message>
git commit -m "prueba_pluggin git"
</commit_message>
<xml_diff>
--- a/Grouped_sales_data.xlsx
+++ b/Grouped_sales_data.xlsx
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>229786700</v>
+        <v>229916300</v>
       </c>
       <c r="E4">
         <v>12000</v>
@@ -531,10 +531,10 @@
         <v>250</v>
       </c>
       <c r="G4">
-        <v>956.5557835844195</v>
+        <v>956.1161729786376</v>
       </c>
       <c r="H4">
-        <v>3401830.35</v>
+        <v>3400179.15</v>
       </c>
       <c r="I4">
         <v>185</v>
@@ -543,10 +543,10 @@
         <v>5.3</v>
       </c>
       <c r="K4">
-        <v>14.22925361709603</v>
+        <v>14.2077275519286</v>
       </c>
       <c r="L4">
-        <v>8057607.5</v>
+        <v>8012040</v>
       </c>
       <c r="M4">
         <v>2400</v>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>33.54219829075484</v>
+        <v>33.31839031226478</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -569,7 +569,7 @@
         <v>17</v>
       </c>
       <c r="D5">
-        <v>142975100</v>
+        <v>142842250</v>
       </c>
       <c r="E5">
         <v>12000</v>
@@ -578,10 +578,10 @@
         <v>250</v>
       </c>
       <c r="G5">
-        <v>955.3838238045599</v>
+        <v>951.2796520997882</v>
       </c>
       <c r="H5">
-        <v>2116549.9</v>
+        <v>2119325.4</v>
       </c>
       <c r="I5">
         <v>185</v>
@@ -590,10 +590,10 @@
         <v>5.3</v>
       </c>
       <c r="K5">
-        <v>14.21533661983182</v>
+        <v>14.18614803807382</v>
       </c>
       <c r="L5">
-        <v>5023972.5</v>
+        <v>5056687.5</v>
       </c>
       <c r="M5">
         <v>2400</v>
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>33.57103480073771</v>
+        <v>33.67577818031673</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -616,7 +616,7 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>71174560</v>
+        <v>70352760</v>
       </c>
       <c r="E6">
         <v>8000</v>
@@ -625,10 +625,10 @@
         <v>120</v>
       </c>
       <c r="G6">
-        <v>590.4201610963177</v>
+        <v>585.887290866846</v>
       </c>
       <c r="H6">
-        <v>7982032.5</v>
+        <v>7909352.5</v>
       </c>
       <c r="I6">
         <v>680</v>
@@ -637,10 +637,10 @@
         <v>27.5</v>
       </c>
       <c r="K6">
-        <v>66.54355492196879</v>
+        <v>66.20145387280915</v>
       </c>
       <c r="L6">
-        <v>2512428</v>
+        <v>2431758</v>
       </c>
       <c r="M6">
         <v>1600</v>
@@ -649,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>20.84154990916557</v>
+        <v>20.25131788239409</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -663,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="D7">
-        <v>57972100</v>
+        <v>57665300</v>
       </c>
       <c r="E7">
         <v>12000</v>
@@ -672,10 +672,10 @@
         <v>250</v>
       </c>
       <c r="G7">
-        <v>1062.596916985905</v>
+        <v>1049.757882472876</v>
       </c>
       <c r="H7">
-        <v>739636.4</v>
+        <v>737291.65</v>
       </c>
       <c r="I7">
         <v>185</v>
@@ -684,10 +684,10 @@
         <v>5.3</v>
       </c>
       <c r="K7">
-        <v>13.62857511378084</v>
+        <v>13.49115553522415</v>
       </c>
       <c r="L7">
-        <v>2011577.5</v>
+        <v>1991650</v>
       </c>
       <c r="M7">
         <v>2400</v>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>36.87111644701871</v>
+        <v>36.25664457875191</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -710,7 +710,7 @@
         <v>18</v>
       </c>
       <c r="D8">
-        <v>43775040</v>
+        <v>43733760</v>
       </c>
       <c r="E8">
         <v>8000</v>
@@ -719,10 +719,10 @@
         <v>120</v>
       </c>
       <c r="G8">
-        <v>587.2769959350139</v>
+        <v>582.5575447570333</v>
       </c>
       <c r="H8">
-        <v>4915228.5</v>
+        <v>4933264.5</v>
       </c>
       <c r="I8">
         <v>680</v>
@@ -731,10 +731,10 @@
         <v>27.5</v>
       </c>
       <c r="K8">
-        <v>66.27870145631069</v>
+        <v>66.04102409638554</v>
       </c>
       <c r="L8">
-        <v>1538786</v>
+        <v>1505326</v>
       </c>
       <c r="M8">
         <v>1600</v>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>20.64403869115496</v>
+        <v>20.0517636402387</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -757,7 +757,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>37811700</v>
+        <v>37662800</v>
       </c>
       <c r="E9">
         <v>12000</v>
@@ -766,10 +766,10 @@
         <v>250</v>
       </c>
       <c r="G9">
-        <v>993.4238873417056</v>
+        <v>994.3973597359736</v>
       </c>
       <c r="H9">
-        <v>595987</v>
+        <v>602963.95</v>
       </c>
       <c r="I9">
         <v>185</v>
@@ -778,10 +778,10 @@
         <v>5.3</v>
       </c>
       <c r="K9">
-        <v>15.74602377807133</v>
+        <v>15.99755777241251</v>
       </c>
       <c r="L9">
-        <v>1332605</v>
+        <v>1318397.5</v>
       </c>
       <c r="M9">
         <v>2400</v>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>35.01142872155956</v>
+        <v>34.80917491749175</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>34096500</v>
+        <v>33654600</v>
       </c>
       <c r="E10">
         <v>12000</v>
@@ -813,10 +813,10 @@
         <v>250</v>
       </c>
       <c r="G10">
-        <v>995.4891827975825</v>
+        <v>988.4166935886517</v>
       </c>
       <c r="H10">
-        <v>539885.1</v>
+        <v>532714.75</v>
       </c>
       <c r="I10">
         <v>185</v>
@@ -825,10 +825,10 @@
         <v>5.3</v>
       </c>
       <c r="K10">
-        <v>15.84867459269044</v>
+        <v>15.72171969070948</v>
       </c>
       <c r="L10">
-        <v>1186612.5</v>
+        <v>1177957.5</v>
       </c>
       <c r="M10">
         <v>2400</v>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>34.64460891652799</v>
+        <v>34.59594995447737</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -851,7 +851,7 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>29328350</v>
+        <v>29586050</v>
       </c>
       <c r="E11">
         <v>12000</v>
@@ -860,10 +860,10 @@
         <v>250</v>
       </c>
       <c r="G11">
-        <v>1071.590120208996</v>
+        <v>1064.055026074447</v>
       </c>
       <c r="H11">
-        <v>370183.4</v>
+        <v>377495.85</v>
       </c>
       <c r="I11">
         <v>185</v>
@@ -872,10 +872,10 @@
         <v>5.3</v>
       </c>
       <c r="K11">
-        <v>13.59818535796937</v>
+        <v>13.65067802126275</v>
       </c>
       <c r="L11">
-        <v>1040222.5</v>
+        <v>1058160</v>
       </c>
       <c r="M11">
         <v>2400</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>38.00732580656948</v>
+        <v>38.05646466462866</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -898,7 +898,7 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>26472800</v>
+        <v>26263100</v>
       </c>
       <c r="E12">
         <v>12000</v>
@@ -907,10 +907,10 @@
         <v>250</v>
       </c>
       <c r="G12">
-        <v>981.3827618164968</v>
+        <v>981.6880349867305</v>
       </c>
       <c r="H12">
-        <v>418915.95</v>
+        <v>421813.25</v>
       </c>
       <c r="I12">
         <v>185</v>
@@ -919,10 +919,10 @@
         <v>5.3</v>
       </c>
       <c r="K12">
-        <v>15.60905991504583</v>
+        <v>15.83858703814959</v>
       </c>
       <c r="L12">
-        <v>919405</v>
+        <v>930417.5</v>
       </c>
       <c r="M12">
         <v>1600</v>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>34.08359592215014</v>
+        <v>34.7780622733899</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -945,7 +945,7 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>19844925</v>
+        <v>19783715</v>
       </c>
       <c r="E13">
         <v>1500</v>
@@ -954,10 +954,10 @@
         <v>35</v>
       </c>
       <c r="G13">
-        <v>123.7808985610299</v>
+        <v>123.6783653515544</v>
       </c>
       <c r="H13">
-        <v>2284486.4</v>
+        <v>2276562.9</v>
       </c>
       <c r="I13">
         <v>155</v>
@@ -966,10 +966,10 @@
         <v>5.9</v>
       </c>
       <c r="K13">
-        <v>14.32154168286169</v>
+        <v>14.30100635094133</v>
       </c>
       <c r="L13">
-        <v>696714.25</v>
+        <v>695066.25</v>
       </c>
       <c r="M13">
         <v>300</v>
@@ -978,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>4.345691198393244</v>
+        <v>4.345223210657598</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -992,7 +992,7 @@
         <v>17</v>
       </c>
       <c r="D14">
-        <v>17225800</v>
+        <v>17171100</v>
       </c>
       <c r="E14">
         <v>12000</v>
@@ -1001,10 +1001,10 @@
         <v>250</v>
       </c>
       <c r="G14">
-        <v>962.1739373289392</v>
+        <v>947.6324503311258</v>
       </c>
       <c r="H14">
-        <v>254131.3</v>
+        <v>258820.1</v>
       </c>
       <c r="I14">
         <v>185</v>
@@ -1013,10 +1013,10 @@
         <v>5.3</v>
       </c>
       <c r="K14">
-        <v>14.25461633385685</v>
+        <v>14.35417336808829</v>
       </c>
       <c r="L14">
-        <v>612965</v>
+        <v>589492.5</v>
       </c>
       <c r="M14">
         <v>2400</v>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>34.2381165167849</v>
+        <v>32.53269867549669</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1039,7 +1039,7 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>17001470</v>
+        <v>16921080</v>
       </c>
       <c r="E15">
         <v>1200</v>
@@ -1048,10 +1048,10 @@
         <v>20</v>
       </c>
       <c r="G15">
-        <v>106.3023728389658</v>
+        <v>105.5818800112314</v>
       </c>
       <c r="H15">
-        <v>1002350.2</v>
+        <v>1002707.15</v>
       </c>
       <c r="I15">
         <v>17</v>
@@ -1060,10 +1060,10 @@
         <v>5.3</v>
       </c>
       <c r="K15">
-        <v>6.29842468723098</v>
+        <v>6.290035568213184</v>
       </c>
       <c r="L15">
-        <v>597053.5</v>
+        <v>590209.75</v>
       </c>
       <c r="M15">
         <v>240</v>
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>3.733100947259824</v>
+        <v>3.682711446666459</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1086,7 +1086,7 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>14421702</v>
+        <v>14413420.5</v>
       </c>
       <c r="E16">
         <v>1500</v>
@@ -1095,10 +1095,10 @@
         <v>25.5</v>
       </c>
       <c r="G16">
-        <v>120.2921202111954</v>
+        <v>120.5034737898169</v>
       </c>
       <c r="H16">
-        <v>755397.7</v>
+        <v>753929.65</v>
       </c>
       <c r="I16">
         <v>23</v>
@@ -1107,10 +1107,10 @@
         <v>5.15</v>
       </c>
       <c r="K16">
-        <v>6.330802624852288</v>
+        <v>6.333148389264564</v>
       </c>
       <c r="L16">
-        <v>509990.675</v>
+        <v>505615.95</v>
       </c>
       <c r="M16">
         <v>300</v>
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>4.253857109492947</v>
+        <v>4.227204665161776</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1133,7 +1133,7 @@
         <v>19</v>
       </c>
       <c r="D17">
-        <v>12418500</v>
+        <v>12298940</v>
       </c>
       <c r="E17">
         <v>1500</v>
@@ -1142,10 +1142,10 @@
         <v>35</v>
       </c>
       <c r="G17">
-        <v>124.2520961319112</v>
+        <v>123.9512617915021</v>
       </c>
       <c r="H17">
-        <v>1427868.2</v>
+        <v>1414775.9</v>
       </c>
       <c r="I17">
         <v>155</v>
@@ -1154,10 +1154,10 @@
         <v>5.9</v>
       </c>
       <c r="K17">
-        <v>14.36010378848069</v>
+        <v>14.32873087089946</v>
       </c>
       <c r="L17">
-        <v>435047.75</v>
+        <v>428338.5</v>
       </c>
       <c r="M17">
         <v>300</v>
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>4.352828027134652</v>
+        <v>4.316884019995163</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1180,7 +1180,7 @@
         <v>20</v>
       </c>
       <c r="D18">
-        <v>10544150</v>
+        <v>10569945</v>
       </c>
       <c r="E18">
         <v>1200</v>
@@ -1189,10 +1189,10 @@
         <v>20</v>
       </c>
       <c r="G18">
-        <v>105.3866989165634</v>
+        <v>105.8158474321754</v>
       </c>
       <c r="H18">
-        <v>626045.35</v>
+        <v>625581</v>
       </c>
       <c r="I18">
         <v>17</v>
@@ -1201,10 +1201,10 @@
         <v>5.3</v>
       </c>
       <c r="K18">
-        <v>6.289068762871064</v>
+        <v>6.294204648354965</v>
       </c>
       <c r="L18">
-        <v>367233.75</v>
+        <v>374369.5</v>
       </c>
       <c r="M18">
         <v>240</v>
@@ -1213,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>3.670428876983968</v>
+        <v>3.747817599359295</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1227,7 +1227,7 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>9079058</v>
+        <v>9051243.5</v>
       </c>
       <c r="E19">
         <v>1500</v>
@@ -1236,10 +1236,10 @@
         <v>25.5</v>
       </c>
       <c r="G19">
-        <v>121.1720474595273</v>
+        <v>121.1225176640617</v>
       </c>
       <c r="H19">
-        <v>472609.3</v>
+        <v>471418.35</v>
       </c>
       <c r="I19">
         <v>23</v>
@@ -1248,10 +1248,10 @@
         <v>5.15</v>
       </c>
       <c r="K19">
-        <v>6.340599970484457</v>
+        <v>6.340614534156478</v>
       </c>
       <c r="L19">
-        <v>318552</v>
+        <v>316712.1</v>
       </c>
       <c r="M19">
         <v>300</v>
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>4.251498124841512</v>
+        <v>4.238198533347607</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1274,7 +1274,7 @@
         <v>18</v>
       </c>
       <c r="D20">
-        <v>8947440</v>
+        <v>8798240</v>
       </c>
       <c r="E20">
         <v>8000</v>
@@ -1283,10 +1283,10 @@
         <v>120</v>
       </c>
       <c r="G20">
-        <v>498.6312973695943</v>
+        <v>491.4668752094738</v>
       </c>
       <c r="H20">
-        <v>1033081.5</v>
+        <v>1020497.5</v>
       </c>
       <c r="I20">
         <v>680</v>
@@ -1295,10 +1295,10 @@
         <v>27.5</v>
       </c>
       <c r="K20">
-        <v>57.89517484868863</v>
+        <v>57.3184396764772</v>
       </c>
       <c r="L20">
-        <v>309588</v>
+        <v>326464</v>
       </c>
       <c r="M20">
         <v>1600</v>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="O20">
-        <v>17.25300936246099</v>
+        <v>18.23617472908055</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1321,7 +1321,7 @@
         <v>19</v>
       </c>
       <c r="D21">
-        <v>8746495</v>
+        <v>8775865</v>
       </c>
       <c r="E21">
         <v>1500</v>
@@ -1330,10 +1330,10 @@
         <v>35</v>
       </c>
       <c r="G21">
-        <v>120.764573495706</v>
+        <v>121.0414051832338</v>
       </c>
       <c r="H21">
-        <v>1000182.9</v>
+        <v>1005624.7</v>
       </c>
       <c r="I21">
         <v>155</v>
@@ -1342,10 +1342,10 @@
         <v>5.9</v>
       </c>
       <c r="K21">
-        <v>13.87928479247325</v>
+        <v>13.93990435264763</v>
       </c>
       <c r="L21">
-        <v>307141.5</v>
+        <v>307280.5</v>
       </c>
       <c r="M21">
         <v>300</v>
@@ -1354,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>4.24076298566813</v>
+        <v>4.238176351323394</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1368,7 +1368,7 @@
         <v>18</v>
       </c>
       <c r="D22">
-        <v>8094360</v>
+        <v>8191240</v>
       </c>
       <c r="E22">
         <v>8000</v>
@@ -1377,10 +1377,10 @@
         <v>120</v>
       </c>
       <c r="G22">
-        <v>497.6244928070823</v>
+        <v>497.9779925831357</v>
       </c>
       <c r="H22">
-        <v>934131</v>
+        <v>945007.5</v>
       </c>
       <c r="I22">
         <v>680</v>
@@ -1389,10 +1389,10 @@
         <v>27.5</v>
       </c>
       <c r="K22">
-        <v>57.73725199332468</v>
+        <v>57.70333394394578</v>
       </c>
       <c r="L22">
-        <v>275760</v>
+        <v>287274</v>
       </c>
       <c r="M22">
         <v>1600</v>
@@ -1401,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>16.95315381777942</v>
+        <v>17.46452671894948</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1415,7 +1415,7 @@
         <v>19</v>
       </c>
       <c r="D23">
-        <v>7925065</v>
+        <v>7814700</v>
       </c>
       <c r="E23">
         <v>1500</v>
@@ -1424,10 +1424,10 @@
         <v>35</v>
       </c>
       <c r="G23">
-        <v>121.1987490250654</v>
+        <v>121.1149512576911</v>
       </c>
       <c r="H23">
-        <v>908184.3</v>
+        <v>894280.1</v>
       </c>
       <c r="I23">
         <v>155</v>
@@ -1436,10 +1436,10 @@
         <v>5.9</v>
       </c>
       <c r="K23">
-        <v>13.95703550023052</v>
+        <v>13.93458871558346</v>
       </c>
       <c r="L23">
-        <v>276935.25</v>
+        <v>273478</v>
       </c>
       <c r="M23">
         <v>300</v>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>4.235196286837236</v>
+        <v>4.238457604265146</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1462,7 +1462,7 @@
         <v>18</v>
       </c>
       <c r="D24">
-        <v>6268480</v>
+        <v>6214760</v>
       </c>
       <c r="E24">
         <v>8000</v>
@@ -1471,10 +1471,10 @@
         <v>120</v>
       </c>
       <c r="G24">
-        <v>497.1433103338885</v>
+        <v>499.1374186812304</v>
       </c>
       <c r="H24">
-        <v>726546</v>
+        <v>718210.5</v>
       </c>
       <c r="I24">
         <v>680</v>
@@ -1483,10 +1483,10 @@
         <v>27.5</v>
       </c>
       <c r="K24">
-        <v>57.92441999521645</v>
+        <v>58.02314590402327</v>
       </c>
       <c r="L24">
-        <v>212072</v>
+        <v>215048</v>
       </c>
       <c r="M24">
         <v>1600</v>
@@ -1495,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>16.81909747006107</v>
+        <v>17.2715444542607</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1509,7 +1509,7 @@
         <v>20</v>
       </c>
       <c r="D25">
-        <v>6178535</v>
+        <v>6197340</v>
       </c>
       <c r="E25">
         <v>1200</v>
@@ -1518,10 +1518,10 @@
         <v>20</v>
       </c>
       <c r="G25">
-        <v>93.945823893442</v>
+        <v>93.47420814479638</v>
       </c>
       <c r="H25">
-        <v>400102.55</v>
+        <v>402557.85</v>
       </c>
       <c r="I25">
         <v>17</v>
@@ -1530,10 +1530,10 @@
         <v>5.3</v>
       </c>
       <c r="K25">
-        <v>6.111795032384211</v>
+        <v>6.106022479068073</v>
       </c>
       <c r="L25">
-        <v>219039.25</v>
+        <v>216067</v>
       </c>
       <c r="M25">
         <v>240</v>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>3.330534310520474</v>
+        <v>3.258929110105581</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1556,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="D26">
-        <v>6136780</v>
+        <v>6022095</v>
       </c>
       <c r="E26">
         <v>1500</v>
@@ -1565,10 +1565,10 @@
         <v>35</v>
       </c>
       <c r="G26">
-        <v>122.003578528827</v>
+        <v>120.5310930088265</v>
       </c>
       <c r="H26">
-        <v>703404.3</v>
+        <v>690601.3</v>
       </c>
       <c r="I26">
         <v>155</v>
@@ -1577,10 +1577,10 @@
         <v>5.9</v>
       </c>
       <c r="K26">
-        <v>14.05262810908001</v>
+        <v>13.8970761057673</v>
       </c>
       <c r="L26">
-        <v>212342.25</v>
+        <v>212180.5</v>
       </c>
       <c r="M26">
         <v>300</v>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>4.221515904572565</v>
+        <v>4.246752596921722</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -1603,7 +1603,7 @@
         <v>20</v>
       </c>
       <c r="D27">
-        <v>5581065</v>
+        <v>5588705</v>
       </c>
       <c r="E27">
         <v>1200</v>
@@ -1612,10 +1612,10 @@
         <v>20</v>
       </c>
       <c r="G27">
-        <v>94.25564074849693</v>
+        <v>94.39582805506292</v>
       </c>
       <c r="H27">
-        <v>359961.2</v>
+        <v>360330.25</v>
       </c>
       <c r="I27">
         <v>17</v>
@@ -1624,10 +1624,10 @@
         <v>5.3</v>
       </c>
       <c r="K27">
-        <v>6.112329557996977</v>
+        <v>6.115065761561307</v>
       </c>
       <c r="L27">
-        <v>193931</v>
+        <v>195657.25</v>
       </c>
       <c r="M27">
         <v>240</v>
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>3.275197595082078</v>
+        <v>3.304741998142049</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1650,7 +1650,7 @@
         <v>18</v>
       </c>
       <c r="D28">
-        <v>5349960</v>
+        <v>5228000</v>
       </c>
       <c r="E28">
         <v>8000</v>
@@ -1659,10 +1659,10 @@
         <v>120</v>
       </c>
       <c r="G28">
-        <v>598.1618962432916</v>
+        <v>584.9183262474827</v>
       </c>
       <c r="H28">
-        <v>596897</v>
+        <v>587048.5</v>
       </c>
       <c r="I28">
         <v>680</v>
@@ -1671,10 +1671,10 @@
         <v>27.5</v>
       </c>
       <c r="K28">
-        <v>67.14251968503937</v>
+        <v>66.00500337306049</v>
       </c>
       <c r="L28">
-        <v>184028</v>
+        <v>187168</v>
       </c>
       <c r="M28">
         <v>1600</v>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="O28">
-        <v>20.57558139534884</v>
+        <v>20.94070261803536</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -1697,7 +1697,7 @@
         <v>20</v>
       </c>
       <c r="D29">
-        <v>4345930</v>
+        <v>4325225</v>
       </c>
       <c r="E29">
         <v>1200</v>
@@ -1706,10 +1706,10 @@
         <v>20</v>
       </c>
       <c r="G29">
-        <v>94.07182129096498</v>
+        <v>93.87561314407257</v>
       </c>
       <c r="H29">
-        <v>281035.9</v>
+        <v>280137.15</v>
       </c>
       <c r="I29">
         <v>17</v>
@@ -1718,10 +1718,10 @@
         <v>5.3</v>
       </c>
       <c r="K29">
-        <v>6.110937398073453</v>
+        <v>6.11079445062496</v>
       </c>
       <c r="L29">
-        <v>153539.75</v>
+        <v>154257.5</v>
       </c>
       <c r="M29">
         <v>240</v>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="O29">
-        <v>3.323515087233214</v>
+        <v>3.348037938967748</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1744,7 +1744,7 @@
         <v>18</v>
       </c>
       <c r="D30">
-        <v>1825200</v>
+        <v>1870480</v>
       </c>
       <c r="E30">
         <v>8000</v>
@@ -1753,10 +1753,10 @@
         <v>120</v>
       </c>
       <c r="G30">
-        <v>384.3335439039798</v>
+        <v>390.0896767466111</v>
       </c>
       <c r="H30">
-        <v>221598</v>
+        <v>228068</v>
       </c>
       <c r="I30">
         <v>680</v>
@@ -1765,19 +1765,19 @@
         <v>27.5</v>
       </c>
       <c r="K30">
-        <v>46.89904761904762</v>
+        <v>47.74293489637848</v>
       </c>
       <c r="L30">
-        <v>64510</v>
+        <v>70540</v>
       </c>
       <c r="M30">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="N30">
         <v>0</v>
       </c>
       <c r="O30">
-        <v>13.58391240261108</v>
+        <v>14.711157455683</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -1791,7 +1791,7 @@
         <v>21</v>
       </c>
       <c r="D31">
-        <v>1685592</v>
+        <v>1695612</v>
       </c>
       <c r="E31">
         <v>1500</v>
@@ -1800,10 +1800,10 @@
         <v>25.5</v>
       </c>
       <c r="G31">
-        <v>161.7805931471351</v>
+        <v>163.3537572254335</v>
       </c>
       <c r="H31">
-        <v>70988.95</v>
+        <v>70949</v>
       </c>
       <c r="I31">
         <v>23</v>
@@ -1812,10 +1812,10 @@
         <v>5.15</v>
       </c>
       <c r="K31">
-        <v>6.847588501977429</v>
+        <v>6.866253750120972</v>
       </c>
       <c r="L31">
-        <v>56873.475</v>
+        <v>60443.1</v>
       </c>
       <c r="M31">
         <v>300</v>
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <v>5.458630866685862</v>
+        <v>5.823034682080925</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1838,7 +1838,7 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <v>1509350</v>
+        <v>1499400</v>
       </c>
       <c r="E32">
         <v>1500</v>
@@ -1847,10 +1847,10 @@
         <v>35</v>
       </c>
       <c r="G32">
-        <v>124.4824742268041</v>
+        <v>122.7406679764244</v>
       </c>
       <c r="H32">
-        <v>174040.9</v>
+        <v>172598.3</v>
       </c>
       <c r="I32">
         <v>155</v>
@@ -1859,19 +1859,19 @@
         <v>5.9</v>
       </c>
       <c r="K32">
-        <v>14.42527144633237</v>
+        <v>14.20094619055455</v>
       </c>
       <c r="L32">
-        <v>52036.5</v>
+        <v>52293.5</v>
       </c>
       <c r="M32">
-        <v>300</v>
+        <v>170</v>
       </c>
       <c r="N32">
         <v>0</v>
       </c>
       <c r="O32">
-        <v>4.291670103092783</v>
+        <v>4.280738375900459</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -1885,7 +1885,7 @@
         <v>20</v>
       </c>
       <c r="D33">
-        <v>1270095</v>
+        <v>1296555</v>
       </c>
       <c r="E33">
         <v>1200</v>
@@ -1894,10 +1894,10 @@
         <v>20</v>
       </c>
       <c r="G33">
-        <v>107.5713559752689</v>
+        <v>106.379635707253</v>
       </c>
       <c r="H33">
-        <v>74177.25</v>
+        <v>76441.45</v>
       </c>
       <c r="I33">
         <v>17</v>
@@ -1906,19 +1906,19 @@
         <v>5.3</v>
       </c>
       <c r="K33">
-        <v>6.314032175689479</v>
+        <v>6.30133129997527</v>
       </c>
       <c r="L33">
-        <v>42853.75</v>
+        <v>45861.5</v>
       </c>
       <c r="M33">
-        <v>170</v>
+        <v>240</v>
       </c>
       <c r="N33">
         <v>0</v>
       </c>
       <c r="O33">
-        <v>3.629520623359024</v>
+        <v>3.762840498851329</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -1932,7 +1932,7 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>1109699.5</v>
+        <v>1088854.5</v>
       </c>
       <c r="E34">
         <v>1500</v>
@@ -1941,10 +1941,10 @@
         <v>25.5</v>
       </c>
       <c r="G34">
-        <v>121.610904109589</v>
+        <v>121.4832645319647</v>
       </c>
       <c r="H34">
-        <v>57591.05</v>
+        <v>56534.95</v>
       </c>
       <c r="I34">
         <v>23</v>
@@ -1953,19 +1953,19 @@
         <v>5.15</v>
       </c>
       <c r="K34">
-        <v>6.347520114625812</v>
+        <v>6.345824447188236</v>
       </c>
       <c r="L34">
-        <v>39276.7</v>
+        <v>36600.825</v>
       </c>
       <c r="M34">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="N34">
         <v>0</v>
       </c>
       <c r="O34">
-        <v>4.304295890410959</v>
+        <v>4.08354624567667</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -1979,7 +1979,7 @@
         <v>18</v>
       </c>
       <c r="D35">
-        <v>893280</v>
+        <v>956240</v>
       </c>
       <c r="E35">
         <v>4000</v>
@@ -1988,10 +1988,10 @@
         <v>120</v>
       </c>
       <c r="G35">
-        <v>375.0125944584383</v>
+        <v>384.6500402252615</v>
       </c>
       <c r="H35">
-        <v>109061.5</v>
+        <v>116436.5</v>
       </c>
       <c r="I35">
         <v>342.5</v>
@@ -2000,10 +2000,10 @@
         <v>27.5</v>
       </c>
       <c r="K35">
-        <v>45.92063157894736</v>
+        <v>47.08309745248686</v>
       </c>
       <c r="L35">
-        <v>28978</v>
+        <v>32518</v>
       </c>
       <c r="M35">
         <v>480</v>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <v>12.16540722082284</v>
+        <v>13.0804505229284</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2026,7 +2026,7 @@
         <v>21</v>
       </c>
       <c r="D36">
-        <v>836793</v>
+        <v>861805.5</v>
       </c>
       <c r="E36">
         <v>1500</v>
@@ -2035,10 +2035,10 @@
         <v>25.5</v>
       </c>
       <c r="G36">
-        <v>159.9986615678776</v>
+        <v>157.7242862371889</v>
       </c>
       <c r="H36">
-        <v>35521.2</v>
+        <v>36956.1</v>
       </c>
       <c r="I36">
         <v>23</v>
@@ -2047,10 +2047,10 @@
         <v>5.15</v>
       </c>
       <c r="K36">
-        <v>6.824438040345821</v>
+        <v>6.802153506350082</v>
       </c>
       <c r="L36">
-        <v>28558.725</v>
+        <v>29803.95</v>
       </c>
       <c r="M36">
         <v>300</v>
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <v>5.460559273422562</v>
+        <v>5.454602855051244</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -2073,7 +2073,7 @@
         <v>20</v>
       </c>
       <c r="D37">
-        <v>806680</v>
+        <v>815520</v>
       </c>
       <c r="E37">
         <v>1200</v>
@@ -2082,10 +2082,10 @@
         <v>20</v>
       </c>
       <c r="G37">
-        <v>143.7419814682823</v>
+        <v>143.5774647887324</v>
       </c>
       <c r="H37">
-        <v>36193</v>
+        <v>36688.3</v>
       </c>
       <c r="I37">
         <v>17</v>
@@ -2094,10 +2094,10 @@
         <v>5.3</v>
       </c>
       <c r="K37">
-        <v>6.480393912264995</v>
+        <v>6.482031802120142</v>
       </c>
       <c r="L37">
-        <v>29048</v>
+        <v>28091</v>
       </c>
       <c r="M37">
         <v>240</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>5.176051318602994</v>
+        <v>4.945598591549296</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -2120,7 +2120,7 @@
         <v>21</v>
       </c>
       <c r="D38">
-        <v>634500</v>
+        <v>642763.5</v>
       </c>
       <c r="E38">
         <v>1500</v>
@@ -2129,10 +2129,10 @@
         <v>25.5</v>
       </c>
       <c r="G38">
-        <v>105.7676279379897</v>
+        <v>107.0202297702298</v>
       </c>
       <c r="H38">
-        <v>36495.95</v>
+        <v>36593.65</v>
       </c>
       <c r="I38">
         <v>23</v>
@@ -2141,19 +2141,19 @@
         <v>5.15</v>
       </c>
       <c r="K38">
-        <v>6.106064915509452</v>
+        <v>6.12138675142188</v>
       </c>
       <c r="L38">
-        <v>21415.875</v>
+        <v>22644.15</v>
       </c>
       <c r="M38">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38">
-        <v>3.569907484580764</v>
+        <v>3.770254745254745</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -2161,46 +2161,46 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39">
-        <v>563118</v>
+        <v>588505</v>
       </c>
       <c r="E39">
         <v>1500</v>
       </c>
       <c r="F39">
-        <v>25.5</v>
+        <v>35</v>
       </c>
       <c r="G39">
-        <v>105.452808988764</v>
+        <v>120.2011846405229</v>
       </c>
       <c r="H39">
-        <v>32382.55</v>
+        <v>66044.39999999999</v>
       </c>
       <c r="I39">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="J39">
-        <v>5.15</v>
+        <v>5.9</v>
       </c>
       <c r="K39">
-        <v>6.099557355434168</v>
+        <v>13.55591133004926</v>
       </c>
       <c r="L39">
-        <v>19555.8</v>
+        <v>19824.25</v>
       </c>
       <c r="M39">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="N39">
         <v>0</v>
       </c>
       <c r="O39">
-        <v>3.662134831460674</v>
+        <v>4.049070669934641</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -2208,46 +2208,46 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D40">
-        <v>556795</v>
+        <v>557526</v>
       </c>
       <c r="E40">
         <v>1500</v>
       </c>
       <c r="F40">
-        <v>35</v>
+        <v>25.5</v>
       </c>
       <c r="G40">
-        <v>117.2446830911771</v>
+        <v>104.2494390426328</v>
       </c>
       <c r="H40">
-        <v>63134.2</v>
+        <v>32414.65</v>
       </c>
       <c r="I40">
-        <v>155</v>
+        <v>23</v>
       </c>
       <c r="J40">
-        <v>5.9</v>
+        <v>5.15</v>
       </c>
       <c r="K40">
-        <v>13.36456392887384</v>
+        <v>6.088401577761082</v>
       </c>
       <c r="L40">
-        <v>19405.75</v>
+        <v>20263.65</v>
       </c>
       <c r="M40">
-        <v>170</v>
+        <v>300</v>
       </c>
       <c r="N40">
         <v>0</v>
       </c>
       <c r="O40">
-        <v>4.08628132238366</v>
+        <v>3.789014584891548</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -2261,7 +2261,7 @@
         <v>21</v>
       </c>
       <c r="D41">
-        <v>451255.5</v>
+        <v>435240</v>
       </c>
       <c r="E41">
         <v>1500</v>
@@ -2270,10 +2270,10 @@
         <v>25.5</v>
       </c>
       <c r="G41">
-        <v>107.7496418338109</v>
+        <v>106.1043393466602</v>
       </c>
       <c r="H41">
-        <v>25525.85</v>
+        <v>24943.7</v>
       </c>
       <c r="I41">
         <v>23</v>
@@ -2282,10 +2282,10 @@
         <v>5.15</v>
       </c>
       <c r="K41">
-        <v>6.12424424184261</v>
+        <v>6.107664054848188</v>
       </c>
       <c r="L41">
-        <v>15766.8</v>
+        <v>16110.9</v>
       </c>
       <c r="M41">
         <v>300</v>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="O41">
-        <v>3.764756446991404</v>
+        <v>3.927571916138469</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2308,7 +2308,7 @@
         <v>20</v>
       </c>
       <c r="D42">
-        <v>397080</v>
+        <v>387720</v>
       </c>
       <c r="E42">
         <v>1200</v>
@@ -2317,10 +2317,10 @@
         <v>20</v>
       </c>
       <c r="G42">
-        <v>144.8140043763676</v>
+        <v>141.6587504567044</v>
       </c>
       <c r="H42">
-        <v>17734.8</v>
+        <v>17571.2</v>
       </c>
       <c r="I42">
         <v>17</v>
@@ -2329,19 +2329,19 @@
         <v>5.3</v>
       </c>
       <c r="K42">
-        <v>6.496263736263736</v>
+        <v>6.462375873482898</v>
       </c>
       <c r="L42">
-        <v>13082</v>
+        <v>13669</v>
       </c>
       <c r="M42">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="N42">
         <v>0</v>
       </c>
       <c r="O42">
-        <v>4.770970094821299</v>
+        <v>4.994154183412496</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2355,7 +2355,7 @@
         <v>19</v>
       </c>
       <c r="D43">
-        <v>266190</v>
+        <v>285080</v>
       </c>
       <c r="E43">
         <v>1500</v>
@@ -2364,10 +2364,10 @@
         <v>35</v>
       </c>
       <c r="G43">
-        <v>114.4411006018917</v>
+        <v>116.788201556739</v>
       </c>
       <c r="H43">
-        <v>29951.6</v>
+        <v>32238.3</v>
       </c>
       <c r="I43">
         <v>155</v>
@@ -2376,19 +2376,19 @@
         <v>5.9</v>
       </c>
       <c r="K43">
-        <v>12.94364736387208</v>
+        <v>13.25043156596794</v>
       </c>
       <c r="L43">
-        <v>9835.25</v>
+        <v>9544.75</v>
       </c>
       <c r="M43">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="N43">
         <v>0</v>
       </c>
       <c r="O43">
-        <v>4.228396388650043</v>
+        <v>3.910180253994265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primera versión operativa y analizada de nuestro generador para SPRINT 7
</commit_message>
<xml_diff>
--- a/Grouped_sales_data.xlsx
+++ b/Grouped_sales_data.xlsx
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>229916300</v>
+        <v>228489050</v>
       </c>
       <c r="E4">
         <v>12000</v>
@@ -531,10 +531,10 @@
         <v>250</v>
       </c>
       <c r="G4">
-        <v>956.1161729786376</v>
+        <v>953.6469876249504</v>
       </c>
       <c r="H4">
-        <v>3400179.15</v>
+        <v>3385805</v>
       </c>
       <c r="I4">
         <v>185</v>
@@ -543,10 +543,10 @@
         <v>5.3</v>
       </c>
       <c r="K4">
-        <v>14.2077275519286</v>
+        <v>14.19922415600755</v>
       </c>
       <c r="L4">
-        <v>8012040</v>
+        <v>7958592.5</v>
       </c>
       <c r="M4">
         <v>2400</v>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>33.31839031226478</v>
+        <v>33.21685552703521</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -569,7 +569,7 @@
         <v>17</v>
       </c>
       <c r="D5">
-        <v>142842250</v>
+        <v>143003400</v>
       </c>
       <c r="E5">
         <v>12000</v>
@@ -578,10 +578,10 @@
         <v>250</v>
       </c>
       <c r="G5">
-        <v>951.2796520997882</v>
+        <v>955.4835433565405</v>
       </c>
       <c r="H5">
-        <v>2119325.4</v>
+        <v>2114228</v>
       </c>
       <c r="I5">
         <v>185</v>
@@ -590,10 +590,10 @@
         <v>5.3</v>
       </c>
       <c r="K5">
-        <v>14.18614803807382</v>
+        <v>14.19926526390726</v>
       </c>
       <c r="L5">
-        <v>5056687.5</v>
+        <v>5007737.5</v>
       </c>
       <c r="M5">
         <v>2400</v>
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>33.67577818031673</v>
+        <v>33.45941964106744</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -616,7 +616,7 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>70352760</v>
+        <v>70506160</v>
       </c>
       <c r="E6">
         <v>8000</v>
@@ -625,10 +625,10 @@
         <v>120</v>
       </c>
       <c r="G6">
-        <v>585.887290866846</v>
+        <v>589.1912489763174</v>
       </c>
       <c r="H6">
-        <v>7909352.5</v>
+        <v>7913623.5</v>
       </c>
       <c r="I6">
         <v>680</v>
@@ -637,10 +637,10 @@
         <v>27.5</v>
       </c>
       <c r="K6">
-        <v>66.20145387280915</v>
+        <v>66.48706994328923</v>
       </c>
       <c r="L6">
-        <v>2431758</v>
+        <v>2483516</v>
       </c>
       <c r="M6">
         <v>1600</v>
@@ -649,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>20.25131788239409</v>
+        <v>20.75373121855832</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -663,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="D7">
-        <v>57665300</v>
+        <v>57478800</v>
       </c>
       <c r="E7">
         <v>12000</v>
@@ -672,10 +672,10 @@
         <v>250</v>
       </c>
       <c r="G7">
-        <v>1049.757882472876</v>
+        <v>1062.454713493531</v>
       </c>
       <c r="H7">
-        <v>737291.65</v>
+        <v>727609.75</v>
       </c>
       <c r="I7">
         <v>185</v>
@@ -684,10 +684,10 @@
         <v>5.3</v>
       </c>
       <c r="K7">
-        <v>13.49115553522415</v>
+        <v>13.51957022612832</v>
       </c>
       <c r="L7">
-        <v>1991650</v>
+        <v>2012052.5</v>
       </c>
       <c r="M7">
         <v>2400</v>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>36.25664457875191</v>
+        <v>37.19135859519408</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -710,7 +710,7 @@
         <v>18</v>
       </c>
       <c r="D8">
-        <v>43733760</v>
+        <v>43920120</v>
       </c>
       <c r="E8">
         <v>8000</v>
@@ -719,10 +719,10 @@
         <v>120</v>
       </c>
       <c r="G8">
-        <v>582.5575447570333</v>
+        <v>588.3393390577487</v>
       </c>
       <c r="H8">
-        <v>4933264.5</v>
+        <v>4938446.5</v>
       </c>
       <c r="I8">
         <v>680</v>
@@ -731,10 +731,10 @@
         <v>27.5</v>
       </c>
       <c r="K8">
-        <v>66.04102409638554</v>
+        <v>66.47435759378659</v>
       </c>
       <c r="L8">
-        <v>1505326</v>
+        <v>1529956</v>
       </c>
       <c r="M8">
         <v>1600</v>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>20.0517636402387</v>
+        <v>20.49478238737592</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -757,7 +757,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>37662800</v>
+        <v>38200400</v>
       </c>
       <c r="E9">
         <v>12000</v>
@@ -766,10 +766,10 @@
         <v>250</v>
       </c>
       <c r="G9">
-        <v>994.3973597359736</v>
+        <v>996.9049296693546</v>
       </c>
       <c r="H9">
-        <v>602963.95</v>
+        <v>601606.65</v>
       </c>
       <c r="I9">
         <v>185</v>
@@ -778,10 +778,10 @@
         <v>5.3</v>
       </c>
       <c r="K9">
-        <v>15.99755777241251</v>
+        <v>15.78150232155505</v>
       </c>
       <c r="L9">
-        <v>1318397.5</v>
+        <v>1354125</v>
       </c>
       <c r="M9">
         <v>2400</v>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>34.80917491749175</v>
+        <v>35.33821341893056</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>33654600</v>
+        <v>33956100</v>
       </c>
       <c r="E10">
         <v>12000</v>
@@ -813,10 +813,10 @@
         <v>250</v>
       </c>
       <c r="G10">
-        <v>988.4166935886517</v>
+        <v>989.7717666948436</v>
       </c>
       <c r="H10">
-        <v>532714.75</v>
+        <v>536122.45</v>
       </c>
       <c r="I10">
         <v>185</v>
@@ -825,10 +825,10 @@
         <v>5.3</v>
       </c>
       <c r="K10">
-        <v>15.72171969070948</v>
+        <v>15.71653523686679</v>
       </c>
       <c r="L10">
-        <v>1177957.5</v>
+        <v>1201240</v>
       </c>
       <c r="M10">
         <v>2400</v>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>34.59594995447737</v>
+        <v>35.01442854228</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -851,7 +851,7 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>29586050</v>
+        <v>29604700</v>
       </c>
       <c r="E11">
         <v>12000</v>
@@ -860,10 +860,10 @@
         <v>250</v>
       </c>
       <c r="G11">
-        <v>1064.055026074447</v>
+        <v>1057.121942510266</v>
       </c>
       <c r="H11">
-        <v>377495.85</v>
+        <v>381504.6</v>
       </c>
       <c r="I11">
         <v>185</v>
@@ -872,10 +872,10 @@
         <v>5.3</v>
       </c>
       <c r="K11">
-        <v>13.65067802126275</v>
+        <v>13.68430001076079</v>
       </c>
       <c r="L11">
-        <v>1058160</v>
+        <v>1023705</v>
       </c>
       <c r="M11">
         <v>2400</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>38.05646466462866</v>
+        <v>36.55436529191216</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -898,7 +898,7 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>26263100</v>
+        <v>26829650</v>
       </c>
       <c r="E12">
         <v>12000</v>
@@ -907,10 +907,10 @@
         <v>250</v>
       </c>
       <c r="G12">
-        <v>981.6880349867305</v>
+        <v>998.7585154301455</v>
       </c>
       <c r="H12">
-        <v>421813.25</v>
+        <v>427840.5</v>
       </c>
       <c r="I12">
         <v>185</v>
@@ -919,19 +919,19 @@
         <v>5.3</v>
       </c>
       <c r="K12">
-        <v>15.83858703814959</v>
+        <v>16.00241247755835</v>
       </c>
       <c r="L12">
-        <v>930417.5</v>
+        <v>938782.5</v>
       </c>
       <c r="M12">
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <v>34.7780622733899</v>
+        <v>34.94704612292</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -945,7 +945,7 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>19783715</v>
+        <v>19817055</v>
       </c>
       <c r="E13">
         <v>1500</v>
@@ -954,10 +954,10 @@
         <v>35</v>
       </c>
       <c r="G13">
-        <v>123.6783653515544</v>
+        <v>124.080714540639</v>
       </c>
       <c r="H13">
-        <v>2276562.9</v>
+        <v>2283805.9</v>
       </c>
       <c r="I13">
         <v>155</v>
@@ -966,10 +966,10 @@
         <v>5.9</v>
       </c>
       <c r="K13">
-        <v>14.30100635094133</v>
+        <v>14.36880056876093</v>
       </c>
       <c r="L13">
-        <v>695066.25</v>
+        <v>696224.25</v>
       </c>
       <c r="M13">
         <v>300</v>
@@ -978,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>4.345223210657598</v>
+        <v>4.359275503878881</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -992,7 +992,7 @@
         <v>17</v>
       </c>
       <c r="D14">
-        <v>17171100</v>
+        <v>17437400</v>
       </c>
       <c r="E14">
         <v>12000</v>
@@ -1001,10 +1001,10 @@
         <v>250</v>
       </c>
       <c r="G14">
-        <v>947.6324503311258</v>
+        <v>955.0030122131551</v>
       </c>
       <c r="H14">
-        <v>258820.1</v>
+        <v>260213.05</v>
       </c>
       <c r="I14">
         <v>185</v>
@@ -1013,10 +1013,10 @@
         <v>5.3</v>
       </c>
       <c r="K14">
-        <v>14.35417336808829</v>
+        <v>14.32339131392084</v>
       </c>
       <c r="L14">
-        <v>589492.5</v>
+        <v>616672.5</v>
       </c>
       <c r="M14">
         <v>2400</v>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>32.53269867549669</v>
+        <v>33.77361848951202</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1039,7 +1039,7 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>16921080</v>
+        <v>16917085</v>
       </c>
       <c r="E15">
         <v>1200</v>
@@ -1048,10 +1048,10 @@
         <v>20</v>
       </c>
       <c r="G15">
-        <v>105.5818800112314</v>
+        <v>105.9795083507699</v>
       </c>
       <c r="H15">
-        <v>1002707.15</v>
+        <v>999674.15</v>
       </c>
       <c r="I15">
         <v>17</v>
@@ -1060,10 +1060,10 @@
         <v>5.3</v>
       </c>
       <c r="K15">
-        <v>6.290035568213184</v>
+        <v>6.296009862765227</v>
       </c>
       <c r="L15">
-        <v>590209.75</v>
+        <v>589130</v>
       </c>
       <c r="M15">
         <v>240</v>
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>3.682711446666459</v>
+        <v>3.690689486675103</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1086,7 +1086,7 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>14413420.5</v>
+        <v>14483627</v>
       </c>
       <c r="E16">
         <v>1500</v>
@@ -1095,10 +1095,10 @@
         <v>25.5</v>
       </c>
       <c r="G16">
-        <v>120.5034737898169</v>
+        <v>120.6335590481664</v>
       </c>
       <c r="H16">
-        <v>753929.65</v>
+        <v>756516.2</v>
       </c>
       <c r="I16">
         <v>23</v>
@@ -1107,10 +1107,10 @@
         <v>5.15</v>
       </c>
       <c r="K16">
-        <v>6.333148389264564</v>
+        <v>6.334336981185789</v>
       </c>
       <c r="L16">
-        <v>505615.95</v>
+        <v>511675.775</v>
       </c>
       <c r="M16">
         <v>300</v>
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>4.227204665161776</v>
+        <v>4.261727384789652</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1133,7 +1133,7 @@
         <v>19</v>
       </c>
       <c r="D17">
-        <v>12298940</v>
+        <v>12364450</v>
       </c>
       <c r="E17">
         <v>1500</v>
@@ -1142,10 +1142,10 @@
         <v>35</v>
       </c>
       <c r="G17">
-        <v>123.9512617915021</v>
+        <v>123.8562942631901</v>
       </c>
       <c r="H17">
-        <v>1414775.9</v>
+        <v>1424620.9</v>
       </c>
       <c r="I17">
         <v>155</v>
@@ -1154,10 +1154,10 @@
         <v>5.9</v>
       </c>
       <c r="K17">
-        <v>14.32873087089946</v>
+        <v>14.342880011276</v>
       </c>
       <c r="L17">
-        <v>428338.5</v>
+        <v>435412.75</v>
       </c>
       <c r="M17">
         <v>300</v>
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>4.316884019995163</v>
+        <v>4.361585811738072</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1180,7 +1180,7 @@
         <v>20</v>
       </c>
       <c r="D18">
-        <v>10569945</v>
+        <v>10542905</v>
       </c>
       <c r="E18">
         <v>1200</v>
@@ -1189,10 +1189,10 @@
         <v>20</v>
       </c>
       <c r="G18">
-        <v>105.8158474321754</v>
+        <v>105.5271902869669</v>
       </c>
       <c r="H18">
-        <v>625581</v>
+        <v>625356.5</v>
       </c>
       <c r="I18">
         <v>17</v>
@@ -1201,10 +1201,10 @@
         <v>5.3</v>
       </c>
       <c r="K18">
-        <v>6.294204648354965</v>
+        <v>6.290173811583416</v>
       </c>
       <c r="L18">
-        <v>374369.5</v>
+        <v>369698.25</v>
       </c>
       <c r="M18">
         <v>240</v>
@@ -1213,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>3.747817599359295</v>
+        <v>3.700423894221626</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1227,7 +1227,7 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>9051243.5</v>
+        <v>8996562.5</v>
       </c>
       <c r="E19">
         <v>1500</v>
@@ -1236,10 +1236,10 @@
         <v>25.5</v>
       </c>
       <c r="G19">
-        <v>121.1225176640617</v>
+        <v>120.9914668423955</v>
       </c>
       <c r="H19">
-        <v>471418.35</v>
+        <v>468936.75</v>
       </c>
       <c r="I19">
         <v>23</v>
@@ -1248,10 +1248,10 @@
         <v>5.15</v>
       </c>
       <c r="K19">
-        <v>6.340614534156478</v>
+        <v>6.339467494017926</v>
       </c>
       <c r="L19">
-        <v>316712.1</v>
+        <v>315230.475</v>
       </c>
       <c r="M19">
         <v>300</v>
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>4.238198533347607</v>
+        <v>4.239418951813548</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1271,43 +1271,43 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>8798240</v>
+        <v>8806490</v>
       </c>
       <c r="E20">
-        <v>8000</v>
+        <v>1500</v>
       </c>
       <c r="F20">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="G20">
-        <v>491.4668752094738</v>
+        <v>121.3483161549909</v>
       </c>
       <c r="H20">
-        <v>1020497.5</v>
+        <v>1006873.9</v>
       </c>
       <c r="I20">
-        <v>680</v>
+        <v>155</v>
       </c>
       <c r="J20">
-        <v>27.5</v>
+        <v>5.9</v>
       </c>
       <c r="K20">
-        <v>57.3184396764772</v>
+        <v>13.94620136570772</v>
       </c>
       <c r="L20">
-        <v>326464</v>
+        <v>305117.5</v>
       </c>
       <c r="M20">
-        <v>1600</v>
+        <v>300</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20">
-        <v>18.23617472908055</v>
+        <v>4.204341894945709</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1318,43 +1318,43 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21">
-        <v>8775865</v>
+        <v>8695600</v>
       </c>
       <c r="E21">
-        <v>1500</v>
+        <v>8000</v>
       </c>
       <c r="F21">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="G21">
-        <v>121.0414051832338</v>
+        <v>486.6032456631226</v>
       </c>
       <c r="H21">
-        <v>1005624.7</v>
+        <v>1013334.5</v>
       </c>
       <c r="I21">
-        <v>155</v>
+        <v>680</v>
       </c>
       <c r="J21">
-        <v>5.9</v>
+        <v>27.5</v>
       </c>
       <c r="K21">
-        <v>13.93990435264763</v>
+        <v>56.9673094220823</v>
       </c>
       <c r="L21">
-        <v>307280.5</v>
+        <v>315326</v>
       </c>
       <c r="M21">
-        <v>300</v>
+        <v>1600</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21">
-        <v>4.238176351323394</v>
+        <v>17.64555120313374</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1368,7 +1368,7 @@
         <v>18</v>
       </c>
       <c r="D22">
-        <v>8191240</v>
+        <v>7927240</v>
       </c>
       <c r="E22">
         <v>8000</v>
@@ -1377,10 +1377,10 @@
         <v>120</v>
       </c>
       <c r="G22">
-        <v>497.9779925831357</v>
+        <v>492.6505499968927</v>
       </c>
       <c r="H22">
-        <v>945007.5</v>
+        <v>918950</v>
       </c>
       <c r="I22">
         <v>680</v>
@@ -1389,10 +1389,10 @@
         <v>27.5</v>
       </c>
       <c r="K22">
-        <v>57.70333394394578</v>
+        <v>57.39133150137397</v>
       </c>
       <c r="L22">
-        <v>287274</v>
+        <v>280790</v>
       </c>
       <c r="M22">
         <v>1600</v>
@@ -1401,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>17.46452671894948</v>
+        <v>17.45012740041017</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1415,7 +1415,7 @@
         <v>19</v>
       </c>
       <c r="D23">
-        <v>7814700</v>
+        <v>7856815</v>
       </c>
       <c r="E23">
         <v>1500</v>
@@ -1424,10 +1424,10 @@
         <v>35</v>
       </c>
       <c r="G23">
-        <v>121.1149512576911</v>
+        <v>121.1648726173586</v>
       </c>
       <c r="H23">
-        <v>894280.1</v>
+        <v>899434.4</v>
       </c>
       <c r="I23">
         <v>155</v>
@@ -1436,10 +1436,10 @@
         <v>5.9</v>
       </c>
       <c r="K23">
-        <v>13.93458871558346</v>
+        <v>13.93737254780426</v>
       </c>
       <c r="L23">
-        <v>273478</v>
+        <v>276670.25</v>
       </c>
       <c r="M23">
         <v>300</v>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>4.238457604265146</v>
+        <v>4.266705477762013</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1456,46 +1456,46 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D24">
-        <v>6214760</v>
+        <v>6336235</v>
       </c>
       <c r="E24">
-        <v>8000</v>
+        <v>1200</v>
       </c>
       <c r="F24">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="G24">
-        <v>499.1374186812304</v>
+        <v>95.34911892615834</v>
       </c>
       <c r="H24">
-        <v>718210.5</v>
+        <v>404893.95</v>
       </c>
       <c r="I24">
-        <v>680</v>
+        <v>17</v>
       </c>
       <c r="J24">
-        <v>27.5</v>
+        <v>5.3</v>
       </c>
       <c r="K24">
-        <v>58.02314590402327</v>
+        <v>6.123622958257713</v>
       </c>
       <c r="L24">
-        <v>215048</v>
+        <v>219586.25</v>
       </c>
       <c r="M24">
-        <v>1600</v>
+        <v>240</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24">
-        <v>17.2715444542607</v>
+        <v>3.304384301686906</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1503,46 +1503,46 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>6197340</v>
+        <v>6327720</v>
       </c>
       <c r="E25">
-        <v>1200</v>
+        <v>8000</v>
       </c>
       <c r="F25">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="G25">
-        <v>93.47420814479638</v>
+        <v>489.3828306264501</v>
       </c>
       <c r="H25">
-        <v>402557.85</v>
+        <v>736849</v>
       </c>
       <c r="I25">
-        <v>17</v>
+        <v>680</v>
       </c>
       <c r="J25">
-        <v>5.3</v>
+        <v>27.5</v>
       </c>
       <c r="K25">
-        <v>6.106022479068073</v>
+        <v>57.24432877563704</v>
       </c>
       <c r="L25">
-        <v>216067</v>
+        <v>223696</v>
       </c>
       <c r="M25">
-        <v>240</v>
+        <v>1600</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25">
-        <v>3.258929110105581</v>
+        <v>17.30054137664347</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1556,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="D26">
-        <v>6022095</v>
+        <v>6188580</v>
       </c>
       <c r="E26">
         <v>1500</v>
@@ -1565,10 +1565,10 @@
         <v>35</v>
       </c>
       <c r="G26">
-        <v>120.5310930088265</v>
+        <v>121.6739412528017</v>
       </c>
       <c r="H26">
-        <v>690601.3</v>
+        <v>708677</v>
       </c>
       <c r="I26">
         <v>155</v>
@@ -1577,10 +1577,10 @@
         <v>5.9</v>
       </c>
       <c r="K26">
-        <v>13.8970761057673</v>
+        <v>14.00409050489082</v>
       </c>
       <c r="L26">
-        <v>212180.5</v>
+        <v>215287.75</v>
       </c>
       <c r="M26">
         <v>300</v>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>4.246752596921722</v>
+        <v>4.232781841060124</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -1603,7 +1603,7 @@
         <v>20</v>
       </c>
       <c r="D27">
-        <v>5588705</v>
+        <v>5542855</v>
       </c>
       <c r="E27">
         <v>1200</v>
@@ -1612,10 +1612,10 @@
         <v>20</v>
       </c>
       <c r="G27">
-        <v>94.39582805506292</v>
+        <v>93.71320607976736</v>
       </c>
       <c r="H27">
-        <v>360330.25</v>
+        <v>359602.2</v>
       </c>
       <c r="I27">
         <v>17</v>
@@ -1624,10 +1624,10 @@
         <v>5.3</v>
       </c>
       <c r="K27">
-        <v>6.115065761561307</v>
+        <v>6.108515517504969</v>
       </c>
       <c r="L27">
-        <v>195657.25</v>
+        <v>193453.5</v>
       </c>
       <c r="M27">
         <v>240</v>
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>3.304741998142049</v>
+        <v>3.270723789879453</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1650,7 +1650,7 @@
         <v>18</v>
       </c>
       <c r="D28">
-        <v>5228000</v>
+        <v>5501960</v>
       </c>
       <c r="E28">
         <v>8000</v>
@@ -1659,10 +1659,10 @@
         <v>120</v>
       </c>
       <c r="G28">
-        <v>584.9183262474827</v>
+        <v>591.3542562338779</v>
       </c>
       <c r="H28">
-        <v>587048.5</v>
+        <v>616172.5</v>
       </c>
       <c r="I28">
         <v>680</v>
@@ -1671,19 +1671,19 @@
         <v>27.5</v>
       </c>
       <c r="K28">
-        <v>66.00500337306049</v>
+        <v>66.5197560185685</v>
       </c>
       <c r="L28">
-        <v>187168</v>
+        <v>200258</v>
       </c>
       <c r="M28">
-        <v>1600</v>
+        <v>800</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
       <c r="O28">
-        <v>20.94070261803536</v>
+        <v>21.52386070507309</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -1697,7 +1697,7 @@
         <v>20</v>
       </c>
       <c r="D29">
-        <v>4325225</v>
+        <v>4402180</v>
       </c>
       <c r="E29">
         <v>1200</v>
@@ -1706,10 +1706,10 @@
         <v>20</v>
       </c>
       <c r="G29">
-        <v>93.87561314407257</v>
+        <v>94.48360233516483</v>
       </c>
       <c r="H29">
-        <v>280137.15</v>
+        <v>283598</v>
       </c>
       <c r="I29">
         <v>17</v>
@@ -1718,10 +1718,10 @@
         <v>5.3</v>
       </c>
       <c r="K29">
-        <v>6.11079445062496</v>
+        <v>6.115320754716981</v>
       </c>
       <c r="L29">
-        <v>154257.5</v>
+        <v>154384.75</v>
       </c>
       <c r="M29">
         <v>240</v>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="O29">
-        <v>3.348037938967748</v>
+        <v>3.313546316964286</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1744,7 +1744,7 @@
         <v>18</v>
       </c>
       <c r="D30">
-        <v>1870480</v>
+        <v>1855000</v>
       </c>
       <c r="E30">
         <v>8000</v>
@@ -1753,10 +1753,10 @@
         <v>120</v>
       </c>
       <c r="G30">
-        <v>390.0896767466111</v>
+        <v>380.7471264367816</v>
       </c>
       <c r="H30">
-        <v>228068</v>
+        <v>226123</v>
       </c>
       <c r="I30">
         <v>680</v>
@@ -1765,10 +1765,10 @@
         <v>27.5</v>
       </c>
       <c r="K30">
-        <v>47.74293489637848</v>
+        <v>46.73894171145101</v>
       </c>
       <c r="L30">
-        <v>70540</v>
+        <v>66224</v>
       </c>
       <c r="M30">
         <v>1600</v>
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="O30">
-        <v>14.711157455683</v>
+        <v>13.5927750410509</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -1791,7 +1791,7 @@
         <v>21</v>
       </c>
       <c r="D31">
-        <v>1695612</v>
+        <v>1633375.5</v>
       </c>
       <c r="E31">
         <v>1500</v>
@@ -1800,10 +1800,10 @@
         <v>25.5</v>
       </c>
       <c r="G31">
-        <v>163.3537572254335</v>
+        <v>159.5716588511137</v>
       </c>
       <c r="H31">
-        <v>70949</v>
+        <v>69554.45</v>
       </c>
       <c r="I31">
         <v>23</v>
@@ -1812,10 +1812,10 @@
         <v>5.15</v>
       </c>
       <c r="K31">
-        <v>6.866253750120972</v>
+        <v>6.82240804315841</v>
       </c>
       <c r="L31">
-        <v>60443.1</v>
+        <v>59061.225</v>
       </c>
       <c r="M31">
         <v>300</v>
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <v>5.823034682080925</v>
+        <v>5.769951641266119</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1838,7 +1838,7 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <v>1499400</v>
+        <v>1488665</v>
       </c>
       <c r="E32">
         <v>1500</v>
@@ -1847,10 +1847,10 @@
         <v>35</v>
       </c>
       <c r="G32">
-        <v>122.7406679764244</v>
+        <v>123.295096902435</v>
       </c>
       <c r="H32">
-        <v>172598.3</v>
+        <v>171712.6</v>
       </c>
       <c r="I32">
         <v>155</v>
@@ -1859,19 +1859,19 @@
         <v>5.9</v>
       </c>
       <c r="K32">
-        <v>14.20094619055455</v>
+        <v>14.29627841145617</v>
       </c>
       <c r="L32">
-        <v>52293.5</v>
+        <v>51466.5</v>
       </c>
       <c r="M32">
-        <v>170</v>
+        <v>300</v>
       </c>
       <c r="N32">
         <v>0</v>
       </c>
       <c r="O32">
-        <v>4.280738375900459</v>
+        <v>4.262589034288554</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -1885,7 +1885,7 @@
         <v>20</v>
       </c>
       <c r="D33">
-        <v>1296555</v>
+        <v>1263600</v>
       </c>
       <c r="E33">
         <v>1200</v>
@@ -1894,10 +1894,10 @@
         <v>20</v>
       </c>
       <c r="G33">
-        <v>106.379635707253</v>
+        <v>106.3815457147668</v>
       </c>
       <c r="H33">
-        <v>76441.45</v>
+        <v>74525.8</v>
       </c>
       <c r="I33">
         <v>17</v>
@@ -1906,10 +1906,10 @@
         <v>5.3</v>
       </c>
       <c r="K33">
-        <v>6.30133129997527</v>
+        <v>6.300794724382821</v>
       </c>
       <c r="L33">
-        <v>45861.5</v>
+        <v>45783</v>
       </c>
       <c r="M33">
         <v>240</v>
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="O33">
-        <v>3.762840498851329</v>
+        <v>3.854436773867655</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -1932,7 +1932,7 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>1088854.5</v>
+        <v>1094555.5</v>
       </c>
       <c r="E34">
         <v>1500</v>
@@ -1941,10 +1941,10 @@
         <v>25.5</v>
       </c>
       <c r="G34">
-        <v>121.4832645319647</v>
+        <v>120.4661567246313</v>
       </c>
       <c r="H34">
-        <v>56534.95</v>
+        <v>57268.35</v>
       </c>
       <c r="I34">
         <v>23</v>
@@ -1953,10 +1953,10 @@
         <v>5.15</v>
       </c>
       <c r="K34">
-        <v>6.345824447188236</v>
+        <v>6.333593231585932</v>
       </c>
       <c r="L34">
-        <v>36600.825</v>
+        <v>37958.125</v>
       </c>
       <c r="M34">
         <v>150</v>
@@ -1965,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>4.08354624567667</v>
+        <v>4.177649680827647</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -1979,31 +1979,31 @@
         <v>18</v>
       </c>
       <c r="D35">
-        <v>956240</v>
+        <v>921480</v>
       </c>
       <c r="E35">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="F35">
         <v>120</v>
       </c>
       <c r="G35">
-        <v>384.6500402252615</v>
+        <v>379.0538872891814</v>
       </c>
       <c r="H35">
-        <v>116436.5</v>
+        <v>112966</v>
       </c>
       <c r="I35">
-        <v>342.5</v>
+        <v>680</v>
       </c>
       <c r="J35">
         <v>27.5</v>
       </c>
       <c r="K35">
-        <v>47.08309745248686</v>
+        <v>46.73810508895325</v>
       </c>
       <c r="L35">
-        <v>32518</v>
+        <v>31638</v>
       </c>
       <c r="M35">
         <v>480</v>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <v>13.0804505229284</v>
+        <v>13.01439736733854</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2026,7 +2026,7 @@
         <v>21</v>
       </c>
       <c r="D36">
-        <v>861805.5</v>
+        <v>878671.5</v>
       </c>
       <c r="E36">
         <v>1500</v>
@@ -2035,10 +2035,10 @@
         <v>25.5</v>
       </c>
       <c r="G36">
-        <v>157.7242862371889</v>
+        <v>161.6988406330512</v>
       </c>
       <c r="H36">
-        <v>36956.1</v>
+        <v>37033.9</v>
       </c>
       <c r="I36">
         <v>23</v>
@@ -2047,10 +2047,10 @@
         <v>5.15</v>
       </c>
       <c r="K36">
-        <v>6.802153506350082</v>
+        <v>6.847984467455621</v>
       </c>
       <c r="L36">
-        <v>29803.95</v>
+        <v>31310.25</v>
       </c>
       <c r="M36">
         <v>300</v>
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <v>5.454602855051244</v>
+        <v>5.761915715863084</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -2073,7 +2073,7 @@
         <v>20</v>
       </c>
       <c r="D37">
-        <v>815520</v>
+        <v>808680</v>
       </c>
       <c r="E37">
         <v>1200</v>
@@ -2082,10 +2082,10 @@
         <v>20</v>
       </c>
       <c r="G37">
-        <v>143.5774647887324</v>
+        <v>142.0231822971549</v>
       </c>
       <c r="H37">
-        <v>36688.3</v>
+        <v>36684</v>
       </c>
       <c r="I37">
         <v>17</v>
@@ -2094,10 +2094,10 @@
         <v>5.3</v>
       </c>
       <c r="K37">
-        <v>6.482031802120142</v>
+        <v>6.466419883659439</v>
       </c>
       <c r="L37">
-        <v>28091</v>
+        <v>28466</v>
       </c>
       <c r="M37">
         <v>240</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>4.945598591549296</v>
+        <v>4.999297506146821</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -2120,7 +2120,7 @@
         <v>21</v>
       </c>
       <c r="D38">
-        <v>642763.5</v>
+        <v>635734.5</v>
       </c>
       <c r="E38">
         <v>1500</v>
@@ -2129,10 +2129,10 @@
         <v>25.5</v>
       </c>
       <c r="G38">
-        <v>107.0202297702298</v>
+        <v>104.6993577075099</v>
       </c>
       <c r="H38">
-        <v>36593.65</v>
+        <v>36778.95</v>
       </c>
       <c r="I38">
         <v>23</v>
@@ -2141,19 +2141,19 @@
         <v>5.15</v>
       </c>
       <c r="K38">
-        <v>6.12138675142188</v>
+        <v>6.093265407554671</v>
       </c>
       <c r="L38">
-        <v>22644.15</v>
+        <v>22902.225</v>
       </c>
       <c r="M38">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38">
-        <v>3.770254745254745</v>
+        <v>3.771776185770751</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -2161,37 +2161,37 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D39">
-        <v>588505</v>
+        <v>568950</v>
       </c>
       <c r="E39">
         <v>1500</v>
       </c>
       <c r="F39">
-        <v>35</v>
+        <v>25.5</v>
       </c>
       <c r="G39">
-        <v>120.2011846405229</v>
+        <v>107.0058303554636</v>
       </c>
       <c r="H39">
-        <v>66044.39999999999</v>
+        <v>32394.5</v>
       </c>
       <c r="I39">
-        <v>155</v>
+        <v>23</v>
       </c>
       <c r="J39">
-        <v>5.9</v>
+        <v>5.15</v>
       </c>
       <c r="K39">
-        <v>13.55591133004926</v>
+        <v>6.120253164556962</v>
       </c>
       <c r="L39">
-        <v>19824.25</v>
+        <v>20154.3</v>
       </c>
       <c r="M39">
         <v>150</v>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="O39">
-        <v>4.049070669934641</v>
+        <v>3.79053977807034</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -2208,46 +2208,46 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D40">
-        <v>557526</v>
+        <v>565575</v>
       </c>
       <c r="E40">
         <v>1500</v>
       </c>
       <c r="F40">
-        <v>25.5</v>
+        <v>35</v>
       </c>
       <c r="G40">
-        <v>104.2494390426328</v>
+        <v>116.7819533347099</v>
       </c>
       <c r="H40">
-        <v>32414.65</v>
+        <v>63800.2</v>
       </c>
       <c r="I40">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="J40">
-        <v>5.15</v>
+        <v>5.9</v>
       </c>
       <c r="K40">
-        <v>6.088401577761082</v>
+        <v>13.22009946125156</v>
       </c>
       <c r="L40">
-        <v>20263.65</v>
+        <v>19584</v>
       </c>
       <c r="M40">
-        <v>300</v>
+        <v>170</v>
       </c>
       <c r="N40">
         <v>0</v>
       </c>
       <c r="O40">
-        <v>3.789014584891548</v>
+        <v>4.043774519925666</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -2261,7 +2261,7 @@
         <v>21</v>
       </c>
       <c r="D41">
-        <v>435240</v>
+        <v>439789.5</v>
       </c>
       <c r="E41">
         <v>1500</v>
@@ -2270,10 +2270,10 @@
         <v>25.5</v>
       </c>
       <c r="G41">
-        <v>106.1043393466602</v>
+        <v>104.7866333095068</v>
       </c>
       <c r="H41">
-        <v>24943.7</v>
+        <v>25426.65</v>
       </c>
       <c r="I41">
         <v>23</v>
@@ -2282,19 +2282,19 @@
         <v>5.15</v>
       </c>
       <c r="K41">
-        <v>6.107664054848188</v>
+        <v>6.093134435657801</v>
       </c>
       <c r="L41">
-        <v>16110.9</v>
+        <v>15348.75</v>
       </c>
       <c r="M41">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="N41">
         <v>0</v>
       </c>
       <c r="O41">
-        <v>3.927571916138469</v>
+        <v>3.657076483202288</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2308,7 +2308,7 @@
         <v>20</v>
       </c>
       <c r="D42">
-        <v>387720</v>
+        <v>401860</v>
       </c>
       <c r="E42">
         <v>1200</v>
@@ -2317,10 +2317,10 @@
         <v>20</v>
       </c>
       <c r="G42">
-        <v>141.6587504567044</v>
+        <v>142.7059659090909</v>
       </c>
       <c r="H42">
-        <v>17571.2</v>
+        <v>18134.9</v>
       </c>
       <c r="I42">
         <v>17</v>
@@ -2329,19 +2329,19 @@
         <v>5.3</v>
       </c>
       <c r="K42">
-        <v>6.462375873482898</v>
+        <v>6.46981805208705</v>
       </c>
       <c r="L42">
-        <v>13669</v>
+        <v>13423</v>
       </c>
       <c r="M42">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="N42">
         <v>0</v>
       </c>
       <c r="O42">
-        <v>4.994154183412496</v>
+        <v>4.766690340909091</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2355,7 +2355,7 @@
         <v>19</v>
       </c>
       <c r="D43">
-        <v>285080</v>
+        <v>278335</v>
       </c>
       <c r="E43">
         <v>1500</v>
@@ -2364,10 +2364,10 @@
         <v>35</v>
       </c>
       <c r="G43">
-        <v>116.788201556739</v>
+        <v>113.0983340105648</v>
       </c>
       <c r="H43">
-        <v>32238.3</v>
+        <v>31964</v>
       </c>
       <c r="I43">
         <v>155</v>
@@ -2376,10 +2376,10 @@
         <v>5.9</v>
       </c>
       <c r="K43">
-        <v>13.25043156596794</v>
+        <v>13.03588907014682</v>
       </c>
       <c r="L43">
-        <v>9544.75</v>
+        <v>9180</v>
       </c>
       <c r="M43">
         <v>150</v>
@@ -2388,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="O43">
-        <v>3.910180253994265</v>
+        <v>3.730190979276717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primera versión operativa del dataset + raw data
</commit_message>
<xml_diff>
--- a/Grouped_sales_data.xlsx
+++ b/Grouped_sales_data.xlsx
@@ -522,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>228489050</v>
+        <v>229483300</v>
       </c>
       <c r="E4">
         <v>12000</v>
@@ -531,10 +531,10 @@
         <v>250</v>
       </c>
       <c r="G4">
-        <v>953.6469876249504</v>
+        <v>956.8941001830532</v>
       </c>
       <c r="H4">
-        <v>3385805</v>
+        <v>3397250.8</v>
       </c>
       <c r="I4">
         <v>185</v>
@@ -543,10 +543,10 @@
         <v>5.3</v>
       </c>
       <c r="K4">
-        <v>14.19922415600755</v>
+        <v>14.23552374646967</v>
       </c>
       <c r="L4">
-        <v>7958592.5</v>
+        <v>8091852.5</v>
       </c>
       <c r="M4">
         <v>2400</v>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>33.21685552703521</v>
+        <v>33.74121740798346</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -569,7 +569,7 @@
         <v>17</v>
       </c>
       <c r="D5">
-        <v>143003400</v>
+        <v>142503350</v>
       </c>
       <c r="E5">
         <v>12000</v>
@@ -578,10 +578,10 @@
         <v>250</v>
       </c>
       <c r="G5">
-        <v>955.4835433565405</v>
+        <v>952.7726704420093</v>
       </c>
       <c r="H5">
-        <v>2114228</v>
+        <v>2117880.4</v>
       </c>
       <c r="I5">
         <v>185</v>
@@ -590,10 +590,10 @@
         <v>5.3</v>
       </c>
       <c r="K5">
-        <v>14.19926526390726</v>
+        <v>14.2285729641847</v>
       </c>
       <c r="L5">
-        <v>5007737.5</v>
+        <v>4967345</v>
       </c>
       <c r="M5">
         <v>2400</v>
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>33.45941964106744</v>
+        <v>33.21150387451777</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -616,7 +616,7 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>70506160</v>
+        <v>70698880</v>
       </c>
       <c r="E6">
         <v>8000</v>
@@ -625,10 +625,10 @@
         <v>120</v>
       </c>
       <c r="G6">
-        <v>589.1912489763174</v>
+        <v>588.6667776852623</v>
       </c>
       <c r="H6">
-        <v>7913623.5</v>
+        <v>7935341</v>
       </c>
       <c r="I6">
         <v>680</v>
@@ -637,10 +637,10 @@
         <v>27.5</v>
       </c>
       <c r="K6">
-        <v>66.48706994328923</v>
+        <v>66.42286991386743</v>
       </c>
       <c r="L6">
-        <v>2483516</v>
+        <v>2478894</v>
       </c>
       <c r="M6">
         <v>1600</v>
@@ -649,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>20.75373121855832</v>
+        <v>20.64024979184013</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -663,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="D7">
-        <v>57478800</v>
+        <v>57842450</v>
       </c>
       <c r="E7">
         <v>12000</v>
@@ -672,10 +672,10 @@
         <v>250</v>
       </c>
       <c r="G7">
-        <v>1062.454713493531</v>
+        <v>1058.920071763328</v>
       </c>
       <c r="H7">
-        <v>727609.75</v>
+        <v>739963.7</v>
       </c>
       <c r="I7">
         <v>185</v>
@@ -684,10 +684,10 @@
         <v>5.3</v>
       </c>
       <c r="K7">
-        <v>13.51957022612832</v>
+        <v>13.61654122886112</v>
       </c>
       <c r="L7">
-        <v>2012052.5</v>
+        <v>2036192.5</v>
       </c>
       <c r="M7">
         <v>2400</v>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>37.19135859519408</v>
+        <v>37.27651764792033</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -710,7 +710,7 @@
         <v>18</v>
       </c>
       <c r="D8">
-        <v>43920120</v>
+        <v>43887640</v>
       </c>
       <c r="E8">
         <v>8000</v>
@@ -719,10 +719,10 @@
         <v>120</v>
       </c>
       <c r="G8">
-        <v>588.3393390577487</v>
+        <v>584.1870990070016</v>
       </c>
       <c r="H8">
-        <v>4938446.5</v>
+        <v>4950217</v>
       </c>
       <c r="I8">
         <v>680</v>
@@ -731,10 +731,10 @@
         <v>27.5</v>
       </c>
       <c r="K8">
-        <v>66.47435759378659</v>
+        <v>66.21035243763794</v>
       </c>
       <c r="L8">
-        <v>1529956</v>
+        <v>1490964</v>
       </c>
       <c r="M8">
         <v>1600</v>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>20.49478238737592</v>
+        <v>19.84617842025397</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -757,7 +757,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>38200400</v>
+        <v>37485500</v>
       </c>
       <c r="E9">
         <v>12000</v>
@@ -766,10 +766,10 @@
         <v>250</v>
       </c>
       <c r="G9">
-        <v>996.9049296693546</v>
+        <v>991.942312781159</v>
       </c>
       <c r="H9">
-        <v>601606.65</v>
+        <v>597101.45</v>
       </c>
       <c r="I9">
         <v>185</v>
@@ -778,10 +778,10 @@
         <v>5.3</v>
       </c>
       <c r="K9">
-        <v>15.78150232155505</v>
+        <v>15.88542753006278</v>
       </c>
       <c r="L9">
-        <v>1354125</v>
+        <v>1299445</v>
       </c>
       <c r="M9">
         <v>2400</v>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>35.33821341893056</v>
+        <v>34.38594866366763</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>33956100</v>
+        <v>33730050</v>
       </c>
       <c r="E10">
         <v>12000</v>
@@ -813,10 +813,10 @@
         <v>250</v>
       </c>
       <c r="G10">
-        <v>989.7717666948436</v>
+        <v>983.8710147886708</v>
       </c>
       <c r="H10">
-        <v>536122.45</v>
+        <v>535569.25</v>
       </c>
       <c r="I10">
         <v>185</v>
@@ -825,10 +825,10 @@
         <v>5.3</v>
       </c>
       <c r="K10">
-        <v>15.71653523686679</v>
+        <v>15.69341723561989</v>
       </c>
       <c r="L10">
-        <v>1201240</v>
+        <v>1194280</v>
       </c>
       <c r="M10">
         <v>2400</v>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>35.01442854228</v>
+        <v>34.83592451069043</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -851,7 +851,7 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>29604700</v>
+        <v>28584950</v>
       </c>
       <c r="E11">
         <v>12000</v>
@@ -860,10 +860,10 @@
         <v>250</v>
       </c>
       <c r="G11">
-        <v>1057.121942510266</v>
+        <v>1062.361095625674</v>
       </c>
       <c r="H11">
-        <v>381504.6</v>
+        <v>360817.3</v>
       </c>
       <c r="I11">
         <v>185</v>
@@ -872,10 +872,10 @@
         <v>5.3</v>
       </c>
       <c r="K11">
-        <v>13.68430001076079</v>
+        <v>13.47338685586258</v>
       </c>
       <c r="L11">
-        <v>1023705</v>
+        <v>1000865</v>
       </c>
       <c r="M11">
         <v>2400</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>36.55436529191216</v>
+        <v>37.19719775523098</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -898,7 +898,7 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>26829650</v>
+        <v>26352400</v>
       </c>
       <c r="E12">
         <v>12000</v>
@@ -907,10 +907,10 @@
         <v>250</v>
       </c>
       <c r="G12">
-        <v>998.7585154301455</v>
+        <v>996.1970286923978</v>
       </c>
       <c r="H12">
-        <v>427840.5</v>
+        <v>417221.75</v>
       </c>
       <c r="I12">
         <v>185</v>
@@ -919,10 +919,10 @@
         <v>5.3</v>
       </c>
       <c r="K12">
-        <v>16.00241247755835</v>
+        <v>15.84466618562965</v>
       </c>
       <c r="L12">
-        <v>938782.5</v>
+        <v>922392.5</v>
       </c>
       <c r="M12">
         <v>2400</v>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>34.94704612292</v>
+        <v>34.86910747363248</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -945,7 +945,7 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>19817055</v>
+        <v>19842605</v>
       </c>
       <c r="E13">
         <v>1500</v>
@@ -954,10 +954,10 @@
         <v>35</v>
       </c>
       <c r="G13">
-        <v>124.080714540639</v>
+        <v>123.6199248658987</v>
       </c>
       <c r="H13">
-        <v>2283805.9</v>
+        <v>2284878.7</v>
       </c>
       <c r="I13">
         <v>155</v>
@@ -966,10 +966,10 @@
         <v>5.9</v>
       </c>
       <c r="K13">
-        <v>14.36880056876093</v>
+        <v>14.30481005208855</v>
       </c>
       <c r="L13">
-        <v>696224.25</v>
+        <v>696447.5</v>
       </c>
       <c r="M13">
         <v>300</v>
@@ -978,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>4.359275503878881</v>
+        <v>4.338885323930149</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -992,7 +992,7 @@
         <v>17</v>
       </c>
       <c r="D14">
-        <v>17437400</v>
+        <v>17756400</v>
       </c>
       <c r="E14">
         <v>12000</v>
@@ -1001,10 +1001,10 @@
         <v>250</v>
       </c>
       <c r="G14">
-        <v>955.0030122131551</v>
+        <v>958.768898488121</v>
       </c>
       <c r="H14">
-        <v>260213.05</v>
+        <v>264007.15</v>
       </c>
       <c r="I14">
         <v>185</v>
@@ -1013,10 +1013,10 @@
         <v>5.3</v>
       </c>
       <c r="K14">
-        <v>14.32339131392084</v>
+        <v>14.33341386611651</v>
       </c>
       <c r="L14">
-        <v>616672.5</v>
+        <v>622852.5</v>
       </c>
       <c r="M14">
         <v>2400</v>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>33.77361848951202</v>
+        <v>33.6313444924406</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1039,7 +1039,7 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>16917085</v>
+        <v>17023665</v>
       </c>
       <c r="E15">
         <v>1200</v>
@@ -1048,10 +1048,10 @@
         <v>20</v>
       </c>
       <c r="G15">
-        <v>105.9795083507699</v>
+        <v>106.3786251241962</v>
       </c>
       <c r="H15">
-        <v>999674.15</v>
+        <v>1003075.4</v>
       </c>
       <c r="I15">
         <v>17</v>
@@ -1060,10 +1060,10 @@
         <v>5.3</v>
       </c>
       <c r="K15">
-        <v>6.296009862765227</v>
+        <v>6.299933425449065</v>
       </c>
       <c r="L15">
-        <v>589130</v>
+        <v>592422.75</v>
       </c>
       <c r="M15">
         <v>240</v>
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>3.690689486675103</v>
+        <v>3.701971205219054</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1086,7 +1086,7 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>14483627</v>
+        <v>14525709</v>
       </c>
       <c r="E16">
         <v>1500</v>
@@ -1095,10 +1095,10 @@
         <v>25.5</v>
       </c>
       <c r="G16">
-        <v>120.6335590481664</v>
+        <v>121.0213537066969</v>
       </c>
       <c r="H16">
-        <v>756516.2</v>
+        <v>756868.25</v>
       </c>
       <c r="I16">
         <v>23</v>
@@ -1107,10 +1107,10 @@
         <v>5.15</v>
       </c>
       <c r="K16">
-        <v>6.334336981185789</v>
+        <v>6.339514109340056</v>
       </c>
       <c r="L16">
-        <v>511675.775</v>
+        <v>507584.3</v>
       </c>
       <c r="M16">
         <v>300</v>
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>4.261727384789652</v>
+        <v>4.228952893539733</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1133,7 +1133,7 @@
         <v>19</v>
       </c>
       <c r="D17">
-        <v>12364450</v>
+        <v>12381265</v>
       </c>
       <c r="E17">
         <v>1500</v>
@@ -1142,10 +1142,10 @@
         <v>35</v>
       </c>
       <c r="G17">
-        <v>123.8562942631901</v>
+        <v>123.9365865865866</v>
       </c>
       <c r="H17">
-        <v>1424620.9</v>
+        <v>1425391.8</v>
       </c>
       <c r="I17">
         <v>155</v>
@@ -1154,10 +1154,10 @@
         <v>5.9</v>
       </c>
       <c r="K17">
-        <v>14.342880011276</v>
+        <v>14.33966922194725</v>
       </c>
       <c r="L17">
-        <v>435412.75</v>
+        <v>434634.5</v>
       </c>
       <c r="M17">
         <v>300</v>
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>4.361585811738072</v>
+        <v>4.350695695695696</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1180,7 +1180,7 @@
         <v>20</v>
       </c>
       <c r="D18">
-        <v>10542905</v>
+        <v>10597265</v>
       </c>
       <c r="E18">
         <v>1200</v>
@@ -1189,10 +1189,10 @@
         <v>20</v>
       </c>
       <c r="G18">
-        <v>105.5271902869669</v>
+        <v>106.0182378422722</v>
       </c>
       <c r="H18">
-        <v>625356.5</v>
+        <v>626119.15</v>
       </c>
       <c r="I18">
         <v>17</v>
@@ -1201,10 +1201,10 @@
         <v>5.3</v>
       </c>
       <c r="K18">
-        <v>6.290173811583416</v>
+        <v>6.29702155263449</v>
       </c>
       <c r="L18">
-        <v>369698.25</v>
+        <v>368313.25</v>
       </c>
       <c r="M18">
         <v>240</v>
@@ -1213,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>3.700423894221626</v>
+        <v>3.68471692827916</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1227,7 +1227,7 @@
         <v>21</v>
       </c>
       <c r="D19">
-        <v>8996562.5</v>
+        <v>9044107</v>
       </c>
       <c r="E19">
         <v>1500</v>
@@ -1236,10 +1236,10 @@
         <v>25.5</v>
       </c>
       <c r="G19">
-        <v>120.9914668423955</v>
+        <v>120.8685082725256</v>
       </c>
       <c r="H19">
-        <v>468936.75</v>
+        <v>471903.1</v>
       </c>
       <c r="I19">
         <v>23</v>
@@ -1248,10 +1248,10 @@
         <v>5.15</v>
       </c>
       <c r="K19">
-        <v>6.339467494017926</v>
+        <v>6.337502350192044</v>
       </c>
       <c r="L19">
-        <v>315230.475</v>
+        <v>313965.925</v>
       </c>
       <c r="M19">
         <v>300</v>
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>4.239418951813548</v>
+        <v>4.195946930211424</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1271,43 +1271,43 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20">
-        <v>8806490</v>
+        <v>8774080</v>
       </c>
       <c r="E20">
-        <v>1500</v>
+        <v>8000</v>
       </c>
       <c r="F20">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="G20">
-        <v>121.3483161549909</v>
+        <v>488.2083240596484</v>
       </c>
       <c r="H20">
-        <v>1006873.9</v>
+        <v>1019678</v>
       </c>
       <c r="I20">
-        <v>155</v>
+        <v>680</v>
       </c>
       <c r="J20">
-        <v>5.9</v>
+        <v>27.5</v>
       </c>
       <c r="K20">
-        <v>13.94620136570772</v>
+        <v>56.98753702565249</v>
       </c>
       <c r="L20">
-        <v>305117.5</v>
+        <v>305968</v>
       </c>
       <c r="M20">
-        <v>300</v>
+        <v>1600</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20">
-        <v>4.204341894945709</v>
+        <v>17.02470509681727</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1318,43 +1318,43 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D21">
-        <v>8695600</v>
+        <v>8731150</v>
       </c>
       <c r="E21">
-        <v>8000</v>
+        <v>1500</v>
       </c>
       <c r="F21">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="G21">
-        <v>486.6032456631226</v>
+        <v>121.0809873803911</v>
       </c>
       <c r="H21">
-        <v>1013334.5</v>
+        <v>998913.1</v>
       </c>
       <c r="I21">
-        <v>680</v>
+        <v>155</v>
       </c>
       <c r="J21">
-        <v>27.5</v>
+        <v>5.9</v>
       </c>
       <c r="K21">
-        <v>56.9673094220823</v>
+        <v>13.92329811552186</v>
       </c>
       <c r="L21">
-        <v>315326</v>
+        <v>304993</v>
       </c>
       <c r="M21">
-        <v>1600</v>
+        <v>300</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21">
-        <v>17.64555120313374</v>
+        <v>4.229552073221467</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1368,7 +1368,7 @@
         <v>18</v>
       </c>
       <c r="D22">
-        <v>7927240</v>
+        <v>8047080</v>
       </c>
       <c r="E22">
         <v>8000</v>
@@ -1377,10 +1377,10 @@
         <v>120</v>
       </c>
       <c r="G22">
-        <v>492.6505499968927</v>
+        <v>492.3869546594872</v>
       </c>
       <c r="H22">
-        <v>918950</v>
+        <v>934669.5</v>
       </c>
       <c r="I22">
         <v>680</v>
@@ -1389,10 +1389,10 @@
         <v>27.5</v>
       </c>
       <c r="K22">
-        <v>57.39133150137397</v>
+        <v>57.52520310192023</v>
       </c>
       <c r="L22">
-        <v>280790</v>
+        <v>274418</v>
       </c>
       <c r="M22">
         <v>1600</v>
@@ -1401,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>17.45012740041017</v>
+        <v>16.79116441289849</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1415,7 +1415,7 @@
         <v>19</v>
       </c>
       <c r="D23">
-        <v>7856815</v>
+        <v>7893935</v>
       </c>
       <c r="E23">
         <v>1500</v>
@@ -1424,10 +1424,10 @@
         <v>35</v>
       </c>
       <c r="G23">
-        <v>121.1648726173586</v>
+        <v>121.7410783134388</v>
       </c>
       <c r="H23">
-        <v>899434.4</v>
+        <v>902367.2000000001</v>
       </c>
       <c r="I23">
         <v>155</v>
@@ -1436,10 +1436,10 @@
         <v>5.9</v>
       </c>
       <c r="K23">
-        <v>13.93737254780426</v>
+        <v>13.98346841053137</v>
       </c>
       <c r="L23">
-        <v>276670.25</v>
+        <v>276509.75</v>
       </c>
       <c r="M23">
         <v>300</v>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>4.266705477762013</v>
+        <v>4.2643618333796</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1462,7 +1462,7 @@
         <v>20</v>
       </c>
       <c r="D24">
-        <v>6336235</v>
+        <v>6228305</v>
       </c>
       <c r="E24">
         <v>1200</v>
@@ -1471,10 +1471,10 @@
         <v>20</v>
       </c>
       <c r="G24">
-        <v>95.34911892615834</v>
+        <v>94.14430823646779</v>
       </c>
       <c r="H24">
-        <v>404893.95</v>
+        <v>402491.05</v>
       </c>
       <c r="I24">
         <v>17</v>
@@ -1483,10 +1483,10 @@
         <v>5.3</v>
       </c>
       <c r="K24">
-        <v>6.123622958257713</v>
+        <v>6.112890512279209</v>
       </c>
       <c r="L24">
-        <v>219586.25</v>
+        <v>217678.5</v>
       </c>
       <c r="M24">
         <v>240</v>
@@ -1495,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>3.304384301686906</v>
+        <v>3.290332088819021</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1509,7 +1509,7 @@
         <v>18</v>
       </c>
       <c r="D25">
-        <v>6327720</v>
+        <v>6223920</v>
       </c>
       <c r="E25">
         <v>8000</v>
@@ -1518,10 +1518,10 @@
         <v>120</v>
       </c>
       <c r="G25">
-        <v>489.3828306264501</v>
+        <v>498.1128451380552</v>
       </c>
       <c r="H25">
-        <v>736849</v>
+        <v>721864</v>
       </c>
       <c r="I25">
         <v>680</v>
@@ -1530,10 +1530,10 @@
         <v>27.5</v>
       </c>
       <c r="K25">
-        <v>57.24432877563704</v>
+        <v>58.02765273311897</v>
       </c>
       <c r="L25">
-        <v>223696</v>
+        <v>218610</v>
       </c>
       <c r="M25">
         <v>1600</v>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>17.30054137664347</v>
+        <v>17.49579831932773</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1556,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="D26">
-        <v>6188580</v>
+        <v>6103475</v>
       </c>
       <c r="E26">
         <v>1500</v>
@@ -1565,10 +1565,10 @@
         <v>35</v>
       </c>
       <c r="G26">
-        <v>121.6739412528017</v>
+        <v>121.840439972851</v>
       </c>
       <c r="H26">
-        <v>708677</v>
+        <v>697164.7000000001</v>
       </c>
       <c r="I26">
         <v>155</v>
@@ -1577,10 +1577,10 @@
         <v>5.9</v>
       </c>
       <c r="K26">
-        <v>14.00409050489082</v>
+        <v>13.98861711946707</v>
       </c>
       <c r="L26">
-        <v>215287.75</v>
+        <v>216904</v>
       </c>
       <c r="M26">
         <v>300</v>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>4.232781841060124</v>
+        <v>4.329939713338923</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -1603,7 +1603,7 @@
         <v>20</v>
       </c>
       <c r="D27">
-        <v>5542855</v>
+        <v>5618155</v>
       </c>
       <c r="E27">
         <v>1200</v>
@@ -1612,10 +1612,10 @@
         <v>20</v>
       </c>
       <c r="G27">
-        <v>93.71320607976736</v>
+        <v>93.91295989836685</v>
       </c>
       <c r="H27">
-        <v>359602.2</v>
+        <v>363723.7</v>
       </c>
       <c r="I27">
         <v>17</v>
@@ -1624,10 +1624,10 @@
         <v>5.3</v>
       </c>
       <c r="K27">
-        <v>6.108515517504969</v>
+        <v>6.110435951280975</v>
       </c>
       <c r="L27">
-        <v>193453.5</v>
+        <v>195038</v>
       </c>
       <c r="M27">
         <v>240</v>
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>3.270723789879453</v>
+        <v>3.260251074001638</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1650,7 +1650,7 @@
         <v>18</v>
       </c>
       <c r="D28">
-        <v>5501960</v>
+        <v>5394400</v>
       </c>
       <c r="E28">
         <v>8000</v>
@@ -1659,10 +1659,10 @@
         <v>120</v>
       </c>
       <c r="G28">
-        <v>591.3542562338779</v>
+        <v>590.0032811987313</v>
       </c>
       <c r="H28">
-        <v>616172.5</v>
+        <v>607782</v>
       </c>
       <c r="I28">
         <v>680</v>
@@ -1671,19 +1671,19 @@
         <v>27.5</v>
       </c>
       <c r="K28">
-        <v>66.5197560185685</v>
+        <v>66.81860158311346</v>
       </c>
       <c r="L28">
-        <v>200258</v>
+        <v>187824</v>
       </c>
       <c r="M28">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
       <c r="O28">
-        <v>21.52386070507309</v>
+        <v>20.54292901673411</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -1697,7 +1697,7 @@
         <v>20</v>
       </c>
       <c r="D29">
-        <v>4402180</v>
+        <v>4375505</v>
       </c>
       <c r="E29">
         <v>1200</v>
@@ -1706,10 +1706,10 @@
         <v>20</v>
       </c>
       <c r="G29">
-        <v>94.48360233516483</v>
+        <v>94.96277888705617</v>
       </c>
       <c r="H29">
-        <v>283598</v>
+        <v>280401.7</v>
       </c>
       <c r="I29">
         <v>17</v>
@@ -1718,10 +1718,10 @@
         <v>5.3</v>
       </c>
       <c r="K29">
-        <v>6.115320754716981</v>
+        <v>6.119902658343882</v>
       </c>
       <c r="L29">
-        <v>154384.75</v>
+        <v>155420</v>
       </c>
       <c r="M29">
         <v>240</v>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="O29">
-        <v>3.313546316964286</v>
+        <v>3.373122666898168</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1744,7 +1744,7 @@
         <v>18</v>
       </c>
       <c r="D30">
-        <v>1855000</v>
+        <v>1855120</v>
       </c>
       <c r="E30">
         <v>8000</v>
@@ -1753,10 +1753,10 @@
         <v>120</v>
       </c>
       <c r="G30">
-        <v>380.7471264367816</v>
+        <v>383.2892561983471</v>
       </c>
       <c r="H30">
-        <v>226123</v>
+        <v>225941</v>
       </c>
       <c r="I30">
         <v>680</v>
@@ -1765,19 +1765,19 @@
         <v>27.5</v>
       </c>
       <c r="K30">
-        <v>46.73894171145101</v>
+        <v>46.91465946843854</v>
       </c>
       <c r="L30">
-        <v>66224</v>
+        <v>66954</v>
       </c>
       <c r="M30">
-        <v>1600</v>
+        <v>800</v>
       </c>
       <c r="N30">
         <v>0</v>
       </c>
       <c r="O30">
-        <v>13.5927750410509</v>
+        <v>13.83347107438017</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -1791,7 +1791,7 @@
         <v>21</v>
       </c>
       <c r="D31">
-        <v>1633375.5</v>
+        <v>1666771.5</v>
       </c>
       <c r="E31">
         <v>1500</v>
@@ -1800,10 +1800,10 @@
         <v>25.5</v>
       </c>
       <c r="G31">
-        <v>159.5716588511137</v>
+        <v>161.0718496327793</v>
       </c>
       <c r="H31">
-        <v>69554.45</v>
+        <v>70343.75</v>
       </c>
       <c r="I31">
         <v>23</v>
@@ -1812,10 +1812,10 @@
         <v>5.15</v>
       </c>
       <c r="K31">
-        <v>6.82240804315841</v>
+        <v>6.837456259720062</v>
       </c>
       <c r="L31">
-        <v>59061.225</v>
+        <v>58258.875</v>
       </c>
       <c r="M31">
         <v>300</v>
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <v>5.769951641266119</v>
+        <v>5.629964727483571</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1838,7 +1838,7 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <v>1488665</v>
+        <v>1516875</v>
       </c>
       <c r="E32">
         <v>1500</v>
@@ -1847,10 +1847,10 @@
         <v>35</v>
       </c>
       <c r="G32">
-        <v>123.295096902435</v>
+        <v>124.4156003937008</v>
       </c>
       <c r="H32">
-        <v>171712.6</v>
+        <v>174086.7</v>
       </c>
       <c r="I32">
         <v>155</v>
@@ -1859,19 +1859,19 @@
         <v>5.9</v>
       </c>
       <c r="K32">
-        <v>14.29627841145617</v>
+        <v>14.34228868017795</v>
       </c>
       <c r="L32">
-        <v>51466.5</v>
+        <v>53378.5</v>
       </c>
       <c r="M32">
-        <v>300</v>
+        <v>170</v>
       </c>
       <c r="N32">
         <v>0</v>
       </c>
       <c r="O32">
-        <v>4.262589034288554</v>
+        <v>4.37815780839895</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -1885,7 +1885,7 @@
         <v>20</v>
       </c>
       <c r="D33">
-        <v>1263600</v>
+        <v>1288850</v>
       </c>
       <c r="E33">
         <v>1200</v>
@@ -1894,10 +1894,10 @@
         <v>20</v>
       </c>
       <c r="G33">
-        <v>106.3815457147668</v>
+        <v>105.9038619556286</v>
       </c>
       <c r="H33">
-        <v>74525.8</v>
+        <v>76315.8</v>
       </c>
       <c r="I33">
         <v>17</v>
@@ -1906,19 +1906,19 @@
         <v>5.3</v>
       </c>
       <c r="K33">
-        <v>6.300794724382821</v>
+        <v>6.298242139143353</v>
       </c>
       <c r="L33">
-        <v>45783</v>
+        <v>46095.25</v>
       </c>
       <c r="M33">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="N33">
         <v>0</v>
       </c>
       <c r="O33">
-        <v>3.854436773867655</v>
+        <v>3.787612982744454</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -1932,7 +1932,7 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <v>1094555.5</v>
+        <v>1092294</v>
       </c>
       <c r="E34">
         <v>1500</v>
@@ -1941,10 +1941,10 @@
         <v>25.5</v>
       </c>
       <c r="G34">
-        <v>120.4661567246313</v>
+        <v>118.5086253661712</v>
       </c>
       <c r="H34">
-        <v>57268.35</v>
+        <v>57816.1</v>
       </c>
       <c r="I34">
         <v>23</v>
@@ -1953,19 +1953,19 @@
         <v>5.15</v>
       </c>
       <c r="K34">
-        <v>6.333593231585932</v>
+        <v>6.309046268005238</v>
       </c>
       <c r="L34">
-        <v>37958.125</v>
+        <v>37038.275</v>
       </c>
       <c r="M34">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="N34">
         <v>0</v>
       </c>
       <c r="O34">
-        <v>4.177649680827647</v>
+        <v>4.018474015406315</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -1979,7 +1979,7 @@
         <v>18</v>
       </c>
       <c r="D35">
-        <v>921480</v>
+        <v>929440</v>
       </c>
       <c r="E35">
         <v>8000</v>
@@ -1988,10 +1988,10 @@
         <v>120</v>
       </c>
       <c r="G35">
-        <v>379.0538872891814</v>
+        <v>389.7023060796646</v>
       </c>
       <c r="H35">
-        <v>112966</v>
+        <v>112431.5</v>
       </c>
       <c r="I35">
         <v>680</v>
@@ -2000,10 +2000,10 @@
         <v>27.5</v>
       </c>
       <c r="K35">
-        <v>46.73810508895325</v>
+        <v>47.3595197978096</v>
       </c>
       <c r="L35">
-        <v>31638</v>
+        <v>36394</v>
       </c>
       <c r="M35">
         <v>480</v>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <v>13.01439736733854</v>
+        <v>15.25953878406709</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2026,7 +2026,7 @@
         <v>21</v>
       </c>
       <c r="D36">
-        <v>878671.5</v>
+        <v>827383.5</v>
       </c>
       <c r="E36">
         <v>1500</v>
@@ -2035,10 +2035,10 @@
         <v>25.5</v>
       </c>
       <c r="G36">
-        <v>161.6988406330512</v>
+        <v>162.2638752696607</v>
       </c>
       <c r="H36">
-        <v>37033.9</v>
+        <v>34754</v>
       </c>
       <c r="I36">
         <v>23</v>
@@ -2047,10 +2047,10 @@
         <v>5.15</v>
       </c>
       <c r="K36">
-        <v>6.847984467455621</v>
+        <v>6.853480575823309</v>
       </c>
       <c r="L36">
-        <v>31310.25</v>
+        <v>28744.95</v>
       </c>
       <c r="M36">
         <v>300</v>
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <v>5.761915715863084</v>
+        <v>5.637370072563248</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -2073,7 +2073,7 @@
         <v>20</v>
       </c>
       <c r="D37">
-        <v>808680</v>
+        <v>813720</v>
       </c>
       <c r="E37">
         <v>1200</v>
@@ -2082,10 +2082,10 @@
         <v>20</v>
       </c>
       <c r="G37">
-        <v>142.0231822971549</v>
+        <v>144.3021812378081</v>
       </c>
       <c r="H37">
-        <v>36684</v>
+        <v>36429.1</v>
       </c>
       <c r="I37">
         <v>17</v>
@@ -2094,10 +2094,10 @@
         <v>5.3</v>
       </c>
       <c r="K37">
-        <v>6.466419883659439</v>
+        <v>6.491286528866714</v>
       </c>
       <c r="L37">
-        <v>28466</v>
+        <v>27564</v>
       </c>
       <c r="M37">
         <v>240</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>4.999297506146821</v>
+        <v>4.888100727079269</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -2120,7 +2120,7 @@
         <v>21</v>
       </c>
       <c r="D38">
-        <v>635734.5</v>
+        <v>629404.5</v>
       </c>
       <c r="E38">
         <v>1500</v>
@@ -2129,10 +2129,10 @@
         <v>25.5</v>
       </c>
       <c r="G38">
-        <v>104.6993577075099</v>
+        <v>104.6913672654691</v>
       </c>
       <c r="H38">
-        <v>36778.95</v>
+        <v>36414.5</v>
       </c>
       <c r="I38">
         <v>23</v>
@@ -2141,19 +2141,19 @@
         <v>5.15</v>
       </c>
       <c r="K38">
-        <v>6.093265407554671</v>
+        <v>6.095497154335454</v>
       </c>
       <c r="L38">
-        <v>22902.225</v>
+        <v>20418</v>
       </c>
       <c r="M38">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38">
-        <v>3.771776185770751</v>
+        <v>3.396207584830339</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -2167,7 +2167,7 @@
         <v>21</v>
       </c>
       <c r="D39">
-        <v>568950</v>
+        <v>560226</v>
       </c>
       <c r="E39">
         <v>1500</v>
@@ -2176,10 +2176,10 @@
         <v>25.5</v>
       </c>
       <c r="G39">
-        <v>107.0058303554636</v>
+        <v>103.8802150936399</v>
       </c>
       <c r="H39">
-        <v>32394.5</v>
+        <v>32628.8</v>
       </c>
       <c r="I39">
         <v>23</v>
@@ -2188,10 +2188,10 @@
         <v>5.15</v>
       </c>
       <c r="K39">
-        <v>6.120253164556962</v>
+        <v>6.078390461997019</v>
       </c>
       <c r="L39">
-        <v>20154.3</v>
+        <v>21738.975</v>
       </c>
       <c r="M39">
         <v>150</v>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="O39">
-        <v>3.79053977807034</v>
+        <v>4.030961431485259</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -2214,7 +2214,7 @@
         <v>19</v>
       </c>
       <c r="D40">
-        <v>565575</v>
+        <v>554290</v>
       </c>
       <c r="E40">
         <v>1500</v>
@@ -2223,10 +2223,10 @@
         <v>35</v>
       </c>
       <c r="G40">
-        <v>116.7819533347099</v>
+        <v>113.8172484599589</v>
       </c>
       <c r="H40">
-        <v>63800.2</v>
+        <v>62886.5</v>
       </c>
       <c r="I40">
         <v>155</v>
@@ -2235,19 +2235,19 @@
         <v>5.9</v>
       </c>
       <c r="K40">
-        <v>13.22009946125156</v>
+        <v>12.96896267271602</v>
       </c>
       <c r="L40">
-        <v>19584</v>
+        <v>19116</v>
       </c>
       <c r="M40">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="N40">
         <v>0</v>
       </c>
       <c r="O40">
-        <v>4.043774519925666</v>
+        <v>3.925256673511293</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -2261,7 +2261,7 @@
         <v>21</v>
       </c>
       <c r="D41">
-        <v>439789.5</v>
+        <v>449196</v>
       </c>
       <c r="E41">
         <v>1500</v>
@@ -2270,10 +2270,10 @@
         <v>25.5</v>
       </c>
       <c r="G41">
-        <v>104.7866333095068</v>
+        <v>108.0577339427472</v>
       </c>
       <c r="H41">
-        <v>25426.65</v>
+        <v>25353.35</v>
       </c>
       <c r="I41">
         <v>23</v>
@@ -2282,10 +2282,10 @@
         <v>5.15</v>
       </c>
       <c r="K41">
-        <v>6.093134435657801</v>
+        <v>6.126957467375544</v>
       </c>
       <c r="L41">
-        <v>15348.75</v>
+        <v>14993.775</v>
       </c>
       <c r="M41">
         <v>150</v>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="O41">
-        <v>3.657076483202288</v>
+        <v>3.606873947558335</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2308,7 +2308,7 @@
         <v>20</v>
       </c>
       <c r="D42">
-        <v>401860</v>
+        <v>411600</v>
       </c>
       <c r="E42">
         <v>1200</v>
@@ -2317,10 +2317,10 @@
         <v>20</v>
       </c>
       <c r="G42">
-        <v>142.7059659090909</v>
+        <v>145.4931071049841</v>
       </c>
       <c r="H42">
-        <v>18134.9</v>
+        <v>18327.1</v>
       </c>
       <c r="I42">
         <v>17</v>
@@ -2329,10 +2329,10 @@
         <v>5.3</v>
       </c>
       <c r="K42">
-        <v>6.46981805208705</v>
+        <v>6.501277048598794</v>
       </c>
       <c r="L42">
-        <v>13423</v>
+        <v>14143</v>
       </c>
       <c r="M42">
         <v>240</v>
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="O42">
-        <v>4.766690340909091</v>
+        <v>4.999293036408625</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2355,7 +2355,7 @@
         <v>19</v>
       </c>
       <c r="D43">
-        <v>278335</v>
+        <v>271740</v>
       </c>
       <c r="E43">
         <v>1500</v>
@@ -2364,10 +2364,10 @@
         <v>35</v>
       </c>
       <c r="G43">
-        <v>113.0983340105648</v>
+        <v>115.5357142857143</v>
       </c>
       <c r="H43">
-        <v>31964</v>
+        <v>31087.7</v>
       </c>
       <c r="I43">
         <v>155</v>
@@ -2376,19 +2376,19 @@
         <v>5.9</v>
       </c>
       <c r="K43">
-        <v>13.03588907014682</v>
+        <v>13.26267064846416</v>
       </c>
       <c r="L43">
-        <v>9180</v>
+        <v>9846.5</v>
       </c>
       <c r="M43">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="N43">
         <v>0</v>
       </c>
       <c r="O43">
-        <v>3.730190979276717</v>
+        <v>4.186437074829932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>